<commit_message>
Added a new set of search terms for the spreadsheet
</commit_message>
<xml_diff>
--- a/data-raw/queries_wg2_ch05.xlsx
+++ b/data-raw/queries_wg2_ch05.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/citationManagement/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C027E715-16E2-1C47-A41C-18F1CEA03816}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428BA2F5-986A-FC42-A2B5-C713F3E4FF5F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="800" windowWidth="27640" windowHeight="19440" activeTab="1" xr2:uid="{AEACCC75-8DEC-AC42-A6C7-72B5A2F10F93}"/>
+    <workbookView xWindow="3580" yWindow="600" windowWidth="27640" windowHeight="19440" activeTab="1" xr2:uid="{AEACCC75-8DEC-AC42-A6C7-72B5A2F10F93}"/>
   </bookViews>
   <sheets>
     <sheet name="Queries" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="863" uniqueCount="746">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="748">
   <si>
     <t>valueChain</t>
   </si>
@@ -5258,6 +5258,12 @@
   </si>
   <si>
     <t>c("cereal", "rice", "maize", "corn", "wheat", "sorghum", "millet",  "buckwheat", "fonio", "rye", "teff")</t>
+  </si>
+  <si>
+    <t>searchStrings.nutrients</t>
+  </si>
+  <si>
+    <t>c("protein", "fat", "carbohydrate*", "fiber", "fibre", "vitamin*", "mineral*")</t>
   </si>
 </sst>
 </file>
@@ -5786,7 +5792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F86CE5-FC64-FA44-BB0B-0B6C961403B7}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A33" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -6624,10 +6630,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B44446-4EFF-1748-B076-59F83F2A5201}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6809,6 +6815,14 @@
       </c>
       <c r="B22" s="21" t="s">
         <v>742</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="20" t="s">
+        <v>746</v>
+      </c>
+      <c r="B23" s="21" t="s">
+        <v>747</v>
       </c>
     </row>
   </sheetData>
@@ -9521,15 +9535,87 @@
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="A287:A288"/>
-    <mergeCell ref="A289:A290"/>
-    <mergeCell ref="A308:A312"/>
-    <mergeCell ref="A277:A278"/>
-    <mergeCell ref="C277:C278"/>
-    <mergeCell ref="A279:A280"/>
-    <mergeCell ref="C279:C280"/>
-    <mergeCell ref="A284:A285"/>
-    <mergeCell ref="C284:C285"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A50:A56"/>
+    <mergeCell ref="C123:C124"/>
+    <mergeCell ref="A125:A126"/>
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="A127:A128"/>
+    <mergeCell ref="C127:C128"/>
+    <mergeCell ref="A129:A136"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="A97:A100"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="A115:A118"/>
+    <mergeCell ref="A123:A124"/>
+    <mergeCell ref="A148:A160"/>
+    <mergeCell ref="A161:A164"/>
+    <mergeCell ref="A165:A169"/>
+    <mergeCell ref="B165:B169"/>
+    <mergeCell ref="A171:A172"/>
+    <mergeCell ref="C171:C172"/>
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="A141:A142"/>
+    <mergeCell ref="A143:A145"/>
+    <mergeCell ref="A146:A147"/>
+    <mergeCell ref="C146:C147"/>
+    <mergeCell ref="A184:A185"/>
+    <mergeCell ref="B184:B185"/>
+    <mergeCell ref="A186:A188"/>
+    <mergeCell ref="B186:B188"/>
+    <mergeCell ref="A189:A190"/>
+    <mergeCell ref="C189:C190"/>
+    <mergeCell ref="A174:A175"/>
+    <mergeCell ref="C174:C175"/>
+    <mergeCell ref="A176:A177"/>
+    <mergeCell ref="C176:C177"/>
+    <mergeCell ref="A180:A181"/>
+    <mergeCell ref="A182:A183"/>
+    <mergeCell ref="B182:B183"/>
+    <mergeCell ref="A199:A201"/>
+    <mergeCell ref="C199:C201"/>
+    <mergeCell ref="A202:A203"/>
+    <mergeCell ref="C202:C203"/>
+    <mergeCell ref="A207:A208"/>
+    <mergeCell ref="C207:C208"/>
+    <mergeCell ref="A191:A192"/>
+    <mergeCell ref="C191:C192"/>
+    <mergeCell ref="A194:A195"/>
+    <mergeCell ref="C194:C195"/>
+    <mergeCell ref="A197:A198"/>
+    <mergeCell ref="C197:C198"/>
+    <mergeCell ref="A217:A218"/>
+    <mergeCell ref="C217:C218"/>
+    <mergeCell ref="A219:A220"/>
+    <mergeCell ref="C219:C220"/>
+    <mergeCell ref="A222:A223"/>
+    <mergeCell ref="B222:B223"/>
+    <mergeCell ref="A209:A210"/>
+    <mergeCell ref="C209:C210"/>
+    <mergeCell ref="A211:A212"/>
+    <mergeCell ref="A213:A214"/>
+    <mergeCell ref="C213:C214"/>
+    <mergeCell ref="A215:A216"/>
+    <mergeCell ref="C215:C216"/>
+    <mergeCell ref="C235:C236"/>
+    <mergeCell ref="A237:A238"/>
+    <mergeCell ref="C237:C238"/>
+    <mergeCell ref="A239:A241"/>
+    <mergeCell ref="A242:A249"/>
+    <mergeCell ref="A250:A253"/>
+    <mergeCell ref="C250:C253"/>
+    <mergeCell ref="A224:A226"/>
+    <mergeCell ref="B224:B226"/>
+    <mergeCell ref="A227:A229"/>
+    <mergeCell ref="B227:B229"/>
+    <mergeCell ref="A230:A234"/>
+    <mergeCell ref="A235:A236"/>
     <mergeCell ref="A267:A268"/>
     <mergeCell ref="C267:C268"/>
     <mergeCell ref="A269:A270"/>
@@ -9544,87 +9630,15 @@
     <mergeCell ref="B261:B263"/>
     <mergeCell ref="A264:A266"/>
     <mergeCell ref="B264:B266"/>
-    <mergeCell ref="C235:C236"/>
-    <mergeCell ref="A237:A238"/>
-    <mergeCell ref="C237:C238"/>
-    <mergeCell ref="A239:A241"/>
-    <mergeCell ref="A242:A249"/>
-    <mergeCell ref="A250:A253"/>
-    <mergeCell ref="C250:C253"/>
-    <mergeCell ref="A224:A226"/>
-    <mergeCell ref="B224:B226"/>
-    <mergeCell ref="A227:A229"/>
-    <mergeCell ref="B227:B229"/>
-    <mergeCell ref="A230:A234"/>
-    <mergeCell ref="A235:A236"/>
-    <mergeCell ref="A217:A218"/>
-    <mergeCell ref="C217:C218"/>
-    <mergeCell ref="A219:A220"/>
-    <mergeCell ref="C219:C220"/>
-    <mergeCell ref="A222:A223"/>
-    <mergeCell ref="B222:B223"/>
-    <mergeCell ref="A209:A210"/>
-    <mergeCell ref="C209:C210"/>
-    <mergeCell ref="A211:A212"/>
-    <mergeCell ref="A213:A214"/>
-    <mergeCell ref="C213:C214"/>
-    <mergeCell ref="A215:A216"/>
-    <mergeCell ref="C215:C216"/>
-    <mergeCell ref="A199:A201"/>
-    <mergeCell ref="C199:C201"/>
-    <mergeCell ref="A202:A203"/>
-    <mergeCell ref="C202:C203"/>
-    <mergeCell ref="A207:A208"/>
-    <mergeCell ref="C207:C208"/>
-    <mergeCell ref="A191:A192"/>
-    <mergeCell ref="C191:C192"/>
-    <mergeCell ref="A194:A195"/>
-    <mergeCell ref="C194:C195"/>
-    <mergeCell ref="A197:A198"/>
-    <mergeCell ref="C197:C198"/>
-    <mergeCell ref="A184:A185"/>
-    <mergeCell ref="B184:B185"/>
-    <mergeCell ref="A186:A188"/>
-    <mergeCell ref="B186:B188"/>
-    <mergeCell ref="A189:A190"/>
-    <mergeCell ref="C189:C190"/>
-    <mergeCell ref="A174:A175"/>
-    <mergeCell ref="C174:C175"/>
-    <mergeCell ref="A176:A177"/>
-    <mergeCell ref="C176:C177"/>
-    <mergeCell ref="A180:A181"/>
-    <mergeCell ref="A182:A183"/>
-    <mergeCell ref="B182:B183"/>
-    <mergeCell ref="A148:A160"/>
-    <mergeCell ref="A161:A164"/>
-    <mergeCell ref="A165:A169"/>
-    <mergeCell ref="B165:B169"/>
-    <mergeCell ref="A171:A172"/>
-    <mergeCell ref="C171:C172"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="A141:A142"/>
-    <mergeCell ref="A143:A145"/>
-    <mergeCell ref="A146:A147"/>
-    <mergeCell ref="C146:C147"/>
-    <mergeCell ref="A127:A128"/>
-    <mergeCell ref="C127:C128"/>
-    <mergeCell ref="A129:A136"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="A97:A100"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="A115:A118"/>
-    <mergeCell ref="A123:A124"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="A50:A56"/>
-    <mergeCell ref="C123:C124"/>
-    <mergeCell ref="A125:A126"/>
-    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="A287:A288"/>
+    <mergeCell ref="A289:A290"/>
+    <mergeCell ref="A308:A312"/>
+    <mergeCell ref="A277:A278"/>
+    <mergeCell ref="C277:C278"/>
+    <mergeCell ref="A279:A280"/>
+    <mergeCell ref="C279:C280"/>
+    <mergeCell ref="A284:A285"/>
+    <mergeCell ref="C284:C285"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
fixed code that points to the ch 5 specific queries
</commit_message>
<xml_diff>
--- a/data-raw/queries_wg2_ch05.xlsx
+++ b/data-raw/queries_wg2_ch05.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/citationManagement/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428BA2F5-986A-FC42-A2B5-C713F3E4FF5F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD1B514-10C0-1E41-87A1-99DB25A8D1E2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="600" windowWidth="27640" windowHeight="19440" activeTab="1" xr2:uid="{AEACCC75-8DEC-AC42-A6C7-72B5A2F10F93}"/>
+    <workbookView xWindow="3580" yWindow="500" windowWidth="27640" windowHeight="19440" xr2:uid="{AEACCC75-8DEC-AC42-A6C7-72B5A2F10F93}"/>
   </bookViews>
   <sheets>
     <sheet name="Queries" sheetId="1" r:id="rId1"/>
@@ -5197,9 +5197,6 @@
     <t xml:space="preserve">c("profit*", "financ*", "econ*", "price", "price variability") </t>
   </si>
   <si>
-    <t>carrot* OR cassava OR potato* OR sweet potatoes* OR turnip* OR yam* OR taro* OR cocoyam* OR onion* OR garlic OR ginger OR leek</t>
-  </si>
-  <si>
     <t>(genet* AND crop*)</t>
   </si>
   <si>
@@ -5264,13 +5261,16 @@
   </si>
   <si>
     <t>c("protein", "fat", "carbohydrate*", "fiber", "fibre", "vitamin*", "mineral*")</t>
+  </si>
+  <si>
+    <t>tuber* OR root OR carrot* OR cassava OR potato* OR sweet potatoes* OR turnip* OR yam* OR taro* OR cocoyam* OR onion* OR garlic OR ginger OR leek</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -5368,6 +5368,12 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF1F497D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -5438,7 +5444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5475,6 +5481,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5792,8 +5799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F86CE5-FC64-FA44-BB0B-0B6C961403B7}">
   <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5892,7 +5899,7 @@
         <v>111</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -5907,7 +5914,7 @@
         <v>113</v>
       </c>
       <c r="E7" s="11" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -5922,7 +5929,7 @@
         <v>175</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -6060,7 +6067,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -6071,8 +6078,8 @@
       <c r="D18" s="6" t="s">
         <v>718</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>725</v>
+      <c r="E18" s="24" t="s">
+        <v>747</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -6177,7 +6184,7 @@
         <v>715</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -6267,7 +6274,7 @@
         <v>118</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -6402,7 +6409,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="48" x14ac:dyDescent="0.2">
@@ -6632,7 +6639,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5B44446-4EFF-1748-B076-59F83F2A5201}">
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -6694,7 +6701,7 @@
         <v>144</v>
       </c>
       <c r="B7" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -6702,7 +6709,7 @@
         <v>145</v>
       </c>
       <c r="B8" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -6771,58 +6778,58 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>730</v>
+      </c>
+      <c r="B17" t="s">
         <v>731</v>
-      </c>
-      <c r="B17" t="s">
-        <v>732</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="B18" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="B19" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
+        <v>736</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>737</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>738</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
+        <v>738</v>
+      </c>
+      <c r="B21" s="19" t="s">
         <v>739</v>
-      </c>
-      <c r="B21" s="19" t="s">
-        <v>740</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
+        <v>740</v>
+      </c>
+      <c r="B22" s="21" t="s">
         <v>741</v>
-      </c>
-      <c r="B22" s="21" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
+        <v>745</v>
+      </c>
+      <c r="B23" s="21" t="s">
         <v>746</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>747</v>
       </c>
     </row>
   </sheetData>
@@ -9535,87 +9542,15 @@
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="A50:A56"/>
-    <mergeCell ref="C123:C124"/>
-    <mergeCell ref="A125:A126"/>
-    <mergeCell ref="C125:C126"/>
-    <mergeCell ref="A127:A128"/>
-    <mergeCell ref="C127:C128"/>
-    <mergeCell ref="A129:A136"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="A97:A100"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="A115:A118"/>
-    <mergeCell ref="A123:A124"/>
-    <mergeCell ref="A148:A160"/>
-    <mergeCell ref="A161:A164"/>
-    <mergeCell ref="A165:A169"/>
-    <mergeCell ref="B165:B169"/>
-    <mergeCell ref="A171:A172"/>
-    <mergeCell ref="C171:C172"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="A141:A142"/>
-    <mergeCell ref="A143:A145"/>
-    <mergeCell ref="A146:A147"/>
-    <mergeCell ref="C146:C147"/>
-    <mergeCell ref="A184:A185"/>
-    <mergeCell ref="B184:B185"/>
-    <mergeCell ref="A186:A188"/>
-    <mergeCell ref="B186:B188"/>
-    <mergeCell ref="A189:A190"/>
-    <mergeCell ref="C189:C190"/>
-    <mergeCell ref="A174:A175"/>
-    <mergeCell ref="C174:C175"/>
-    <mergeCell ref="A176:A177"/>
-    <mergeCell ref="C176:C177"/>
-    <mergeCell ref="A180:A181"/>
-    <mergeCell ref="A182:A183"/>
-    <mergeCell ref="B182:B183"/>
-    <mergeCell ref="A199:A201"/>
-    <mergeCell ref="C199:C201"/>
-    <mergeCell ref="A202:A203"/>
-    <mergeCell ref="C202:C203"/>
-    <mergeCell ref="A207:A208"/>
-    <mergeCell ref="C207:C208"/>
-    <mergeCell ref="A191:A192"/>
-    <mergeCell ref="C191:C192"/>
-    <mergeCell ref="A194:A195"/>
-    <mergeCell ref="C194:C195"/>
-    <mergeCell ref="A197:A198"/>
-    <mergeCell ref="C197:C198"/>
-    <mergeCell ref="A217:A218"/>
-    <mergeCell ref="C217:C218"/>
-    <mergeCell ref="A219:A220"/>
-    <mergeCell ref="C219:C220"/>
-    <mergeCell ref="A222:A223"/>
-    <mergeCell ref="B222:B223"/>
-    <mergeCell ref="A209:A210"/>
-    <mergeCell ref="C209:C210"/>
-    <mergeCell ref="A211:A212"/>
-    <mergeCell ref="A213:A214"/>
-    <mergeCell ref="C213:C214"/>
-    <mergeCell ref="A215:A216"/>
-    <mergeCell ref="C215:C216"/>
-    <mergeCell ref="C235:C236"/>
-    <mergeCell ref="A237:A238"/>
-    <mergeCell ref="C237:C238"/>
-    <mergeCell ref="A239:A241"/>
-    <mergeCell ref="A242:A249"/>
-    <mergeCell ref="A250:A253"/>
-    <mergeCell ref="C250:C253"/>
-    <mergeCell ref="A224:A226"/>
-    <mergeCell ref="B224:B226"/>
-    <mergeCell ref="A227:A229"/>
-    <mergeCell ref="B227:B229"/>
-    <mergeCell ref="A230:A234"/>
-    <mergeCell ref="A235:A236"/>
+    <mergeCell ref="A287:A288"/>
+    <mergeCell ref="A289:A290"/>
+    <mergeCell ref="A308:A312"/>
+    <mergeCell ref="A277:A278"/>
+    <mergeCell ref="C277:C278"/>
+    <mergeCell ref="A279:A280"/>
+    <mergeCell ref="C279:C280"/>
+    <mergeCell ref="A284:A285"/>
+    <mergeCell ref="C284:C285"/>
     <mergeCell ref="A267:A268"/>
     <mergeCell ref="C267:C268"/>
     <mergeCell ref="A269:A270"/>
@@ -9630,15 +9565,87 @@
     <mergeCell ref="B261:B263"/>
     <mergeCell ref="A264:A266"/>
     <mergeCell ref="B264:B266"/>
-    <mergeCell ref="A287:A288"/>
-    <mergeCell ref="A289:A290"/>
-    <mergeCell ref="A308:A312"/>
-    <mergeCell ref="A277:A278"/>
-    <mergeCell ref="C277:C278"/>
-    <mergeCell ref="A279:A280"/>
-    <mergeCell ref="C279:C280"/>
-    <mergeCell ref="A284:A285"/>
-    <mergeCell ref="C284:C285"/>
+    <mergeCell ref="C235:C236"/>
+    <mergeCell ref="A237:A238"/>
+    <mergeCell ref="C237:C238"/>
+    <mergeCell ref="A239:A241"/>
+    <mergeCell ref="A242:A249"/>
+    <mergeCell ref="A250:A253"/>
+    <mergeCell ref="C250:C253"/>
+    <mergeCell ref="A224:A226"/>
+    <mergeCell ref="B224:B226"/>
+    <mergeCell ref="A227:A229"/>
+    <mergeCell ref="B227:B229"/>
+    <mergeCell ref="A230:A234"/>
+    <mergeCell ref="A235:A236"/>
+    <mergeCell ref="A217:A218"/>
+    <mergeCell ref="C217:C218"/>
+    <mergeCell ref="A219:A220"/>
+    <mergeCell ref="C219:C220"/>
+    <mergeCell ref="A222:A223"/>
+    <mergeCell ref="B222:B223"/>
+    <mergeCell ref="A209:A210"/>
+    <mergeCell ref="C209:C210"/>
+    <mergeCell ref="A211:A212"/>
+    <mergeCell ref="A213:A214"/>
+    <mergeCell ref="C213:C214"/>
+    <mergeCell ref="A215:A216"/>
+    <mergeCell ref="C215:C216"/>
+    <mergeCell ref="A199:A201"/>
+    <mergeCell ref="C199:C201"/>
+    <mergeCell ref="A202:A203"/>
+    <mergeCell ref="C202:C203"/>
+    <mergeCell ref="A207:A208"/>
+    <mergeCell ref="C207:C208"/>
+    <mergeCell ref="A191:A192"/>
+    <mergeCell ref="C191:C192"/>
+    <mergeCell ref="A194:A195"/>
+    <mergeCell ref="C194:C195"/>
+    <mergeCell ref="A197:A198"/>
+    <mergeCell ref="C197:C198"/>
+    <mergeCell ref="A184:A185"/>
+    <mergeCell ref="B184:B185"/>
+    <mergeCell ref="A186:A188"/>
+    <mergeCell ref="B186:B188"/>
+    <mergeCell ref="A189:A190"/>
+    <mergeCell ref="C189:C190"/>
+    <mergeCell ref="A174:A175"/>
+    <mergeCell ref="C174:C175"/>
+    <mergeCell ref="A176:A177"/>
+    <mergeCell ref="C176:C177"/>
+    <mergeCell ref="A180:A181"/>
+    <mergeCell ref="A182:A183"/>
+    <mergeCell ref="B182:B183"/>
+    <mergeCell ref="A148:A160"/>
+    <mergeCell ref="A161:A164"/>
+    <mergeCell ref="A165:A169"/>
+    <mergeCell ref="B165:B169"/>
+    <mergeCell ref="A171:A172"/>
+    <mergeCell ref="C171:C172"/>
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="A141:A142"/>
+    <mergeCell ref="A143:A145"/>
+    <mergeCell ref="A146:A147"/>
+    <mergeCell ref="C146:C147"/>
+    <mergeCell ref="A127:A128"/>
+    <mergeCell ref="C127:C128"/>
+    <mergeCell ref="A129:A136"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="A97:A100"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="A115:A118"/>
+    <mergeCell ref="A123:A124"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A50:A56"/>
+    <mergeCell ref="C123:C124"/>
+    <mergeCell ref="A125:A126"/>
+    <mergeCell ref="C125:C126"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Minor tweaks to code and more edits to queries
</commit_message>
<xml_diff>
--- a/data-raw/queries_wg2_ch05.xlsx
+++ b/data-raw/queries_wg2_ch05.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/citationManagement/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A9F484-6A0C-9D44-85FF-B674ADCC148E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3030757C-9F3D-364F-9CAC-9899EA0075ED}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33600" yWindow="0" windowWidth="32240" windowHeight="18220" xr2:uid="{AEACCC75-8DEC-AC42-A6C7-72B5A2F10F93}"/>
+    <workbookView xWindow="-32240" yWindow="0" windowWidth="32240" windowHeight="18220" xr2:uid="{AEACCC75-8DEC-AC42-A6C7-72B5A2F10F93}"/>
   </bookViews>
   <sheets>
     <sheet name="Queries" sheetId="1" r:id="rId1"/>
@@ -5205,9 +5205,6 @@
     <t>heatTolerance</t>
   </si>
   <si>
-    <t>fiber OR fibre OR cotton OR wool OR flax OR silk OR linen OR cashmere OR  camel OR  angora OR alpaca OR vicuna OR mohair OR abaca OR kapok OR hemp OR jute OR rayon OR sisal")c("cotton OR wool OR flax OR silk OR linen OR cashmere OR  camel OR  angora OR alpaca OR vicuna OR mohair OR abaca OR kapok OR hemp OR jute OR rayon OR sisal</t>
-  </si>
-  <si>
     <t>5.13 Climate change and Food Security, Consumption and Nutrition</t>
   </si>
   <si>
@@ -5232,18 +5229,12 @@
     <t>5.14 Competition for and Tradeoffs of Use of Land and Ocean</t>
   </si>
   <si>
-    <t>5.1   Methodologies and Associated Uncertainties</t>
-  </si>
-  <si>
     <t>(indigenous OR local) AND knowledge</t>
   </si>
   <si>
     <t>stress AND human AND ("thermal heat index" OR "temperature humidity index" OR "wet bulb temperature" OR "web bulb globe temperature" OR "heat stress index")</t>
   </si>
   <si>
-    <t>"price vol*" OR "price var*" OR "price uncertain*" OR "agricultural price var*" OR "agricultural price uncertain*" OR  "commodity price var*" OR "commodity price uncertain*"  OR "commodity price vol*"</t>
-  </si>
-  <si>
     <t>agriculture AND (SSP OR "shared socioeconomic profile*" OR RCP OR "representative concentration pathway")</t>
   </si>
   <si>
@@ -5271,24 +5262,15 @@
     <t>(food OR agriculture) AND adaptation OR "adaptive capacity" OR "risk sharing" OR "risk spreading"</t>
   </si>
   <si>
-    <t>(food OR agriculture) AND "social protection" OR migration OR "climate services" OR "climate information" or insurance</t>
-  </si>
-  <si>
     <t>"crop insurance" OR "index insurance"</t>
   </si>
   <si>
-    <t>("free air carbon dioxide" OR  "free air carbon ozone" OR FACE) AND experiment*</t>
-  </si>
-  <si>
     <t>"cropping system" AND (intercrop OR "sequential crop" OR "relay crop" OR "multi* crop" OR "crop rotation" OR "mix tree-crop*" OR "traditional crop" OR "indigenous crop" OR perennial OR "minor crop")</t>
   </si>
   <si>
     <t>"grain quality" OR "nutrient composition"</t>
   </si>
   <si>
-    <t>flood  OR "sea level rise" OR "extreme event" AND crop* AND impact*</t>
-  </si>
-  <si>
     <t>stress AND crop AND (THI OR "thermal heat index" OR "temperature humidity index" OR "heat stress index")</t>
   </si>
   <si>
@@ -5328,15 +5310,9 @@
     <t>adapt* AND ("*forest management" OR agroforestry OR agriforestry OR afforestation)</t>
   </si>
   <si>
-    <t>(global OR international) AND (wood OR forestry OR "forest products" trade)</t>
-  </si>
-  <si>
     <t>"medicinal plant*" OR "wild edible*" OR "aquatic algae" OR "aromatic plant*" OR seaweed*</t>
   </si>
   <si>
-    <t xml:space="preserve">"wild food*"  OR  "edible wild plant*"  OR  bushmeat </t>
-  </si>
-  <si>
     <t>Fisheries OR fishing OR "fish resource" OR "fish product*"</t>
   </si>
   <si>
@@ -5424,9 +5400,6 @@
     <t>Fiber</t>
   </si>
   <si>
-    <t>"perennial fruit" OR '"fruit tree" OR orchard* OR apple* OR "Malus pumila" OR apricot* OR citrus OR orange* OR lemon* OR lime* OR grapefruit* OR tangerine* OR mandarin* OR clementine* OR satsuma* OR peach* OR nectarine* OR pear* OR plum* OR quince* OR sloe* OR cherr* OR avocado* OR breadfruit* OR mango*  OR olive* OR "Olea europaea" OR guava* OR lyche* OR jackfruit* OR "dragon fruit*" OR "palm fruit*" OR kapok OR banana* OR plantain* OR Musa OR grape* OR "kiwi fruit" OR "Vitis vinifera" OR "date palm" OR "Phoenix dactylifera" OR "common fig" OR "Ficus carica"</t>
-  </si>
-  <si>
     <t>"rubber tree" OR "rubber crop" OR latex OR "Hevea brasiliensis" OR "maple syrup" OR coconut OR "Cocos nucifera" OR "palm oil" OR "Elaeis guineensis"</t>
   </si>
   <si>
@@ -5445,15 +5418,9 @@
     <t xml:space="preserve">spice* OR chillie* OR chili* OR nutmeg* OR mace OR cardamon* OR cinnamon* OR canella OR clove* OR vanilla* OR "mustard seed" OR anise OR badian OR fennel OR coriander OR "black pepper" OR piper OR sage OR rosemary </t>
   </si>
   <si>
-    <t>tea  OR "Camellia sinensis" OR mate OR "Ilex paraguayensis" OR hops OR tobacco OR cannabis</t>
-  </si>
-  <si>
     <t>ornamental OR floriculture OR "cut flower" OR Pyrethrum</t>
   </si>
   <si>
-    <t>fiber OR fibre OR cotton  OR hemp OR  "common flax" OR  "Linum usitatissimum" OR jute OR Corchorus OR bastfibre* OR sisal OR "agave fiber*" OR "Manila fibre" or "Manila hemp" OR Ramie OR "Boehmeria nivea"</t>
-  </si>
-  <si>
     <t>animalFibre</t>
   </si>
   <si>
@@ -5481,7 +5448,40 @@
     <t>pig OR hog OR swine OR poultry OR chicken OR broilers OR ruminant OR sheep OR goat OR cattle OR buffalo OR beef OR pork OR lamb OR mutton</t>
   </si>
   <si>
-    <t>food AND (nutrition* OR "nutrition* status" OR "nutrition* outcome*" OR nutrient OR  "nutrition* health" OR anthropometry OR diet)</t>
+    <t>food AND (nutrition* OR "nutrition* status" OR "nutrition* outcome*" OR nutrient OR "nutrition* health" OR anthropometry OR diet)</t>
+  </si>
+  <si>
+    <t>(food OR agriculture) AND "social protection" OR migration OR "climate services" OR "climate information" OR insurance</t>
+  </si>
+  <si>
+    <t>("free air carbon dioxide" OR "free air carbon ozone" OR FACE) AND experiment*</t>
+  </si>
+  <si>
+    <t>flood OR "sea level rise" OR "extreme event" AND crop* AND impact*</t>
+  </si>
+  <si>
+    <t>tea OR "Camellia sinensis" OR mate OR "Ilex paraguayensis" OR hops OR tobacco OR cannabis</t>
+  </si>
+  <si>
+    <t>"price vol*" OR "price var*" OR "price uncertain*" OR "agricultural price var*" OR "agricultural price uncertain*" OR "commodity price var*" OR "commodity price uncertain*" OR "commodity price vol*"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"wild food*" OR "edible wild plant*" OR bushmeat </t>
+  </si>
+  <si>
+    <t>5.1 Methodologies and Associated Uncertainties</t>
+  </si>
+  <si>
+    <t>(global OR international) AND (wood OR forestry OR "forest products trade")</t>
+  </si>
+  <si>
+    <t>wool OR silk OR cashmere OR camel OR angora OR alpaca OR vicuna OR mohair</t>
+  </si>
+  <si>
+    <t>cotton OR hemp OR "common flax" OR "Linum usitatissimum" OR jute OR Corchorus OR bastfibre* OR sisal OR "agave fiber*" OR "Manila fibre" OR "Manila hemp" OR ramie OR "Boehmeria nivea"</t>
+  </si>
+  <si>
+    <t>"perennial fruit" OR apple* OR "Malus pumila" OR apricot* OR citrus OR orange* OR lemon* OR lime* OR grapefruit* OR tangerine* OR mandarin* OR clementine* OR satsuma* OR peach* OR nectarine* OR pear* OR plum* OR quince* OR sloe* OR cherr* OR avocado* OR breadfruit* OR mango* OR olive* OR "Olea europaea" OR guava* OR lyche* OR jackfruit* OR "dragon fruit*" OR "palm fruit*" OR kapok OR banana* OR plantain* OR Musa OR grape* OR "kiwi fruit" OR "Vitis vinifera" OR "date palm" OR "Phoenix dactylifera" OR "common fig" OR "Ficus carica"</t>
   </si>
 </sst>
 </file>
@@ -5595,7 +5595,7 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -5603,7 +5603,7 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -5713,9 +5713,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5735,21 +5732,24 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -6067,1215 +6067,1216 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F86CE5-FC64-FA44-BB0B-0B6C961403B7}">
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B82" sqref="B82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="17"/>
+    <col min="1" max="1" width="10.83203125" style="28"/>
     <col min="2" max="2" width="37.6640625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="20" style="20" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" style="20"/>
+    <col min="3" max="3" width="20" style="19" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="19" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="19"/>
+    <col min="6" max="16384" width="10.83203125" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
         <v>85</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="17">
+      <c r="A2" s="28">
         <v>1</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>736</v>
-      </c>
-      <c r="D2" s="20" t="s">
+      <c r="B2" s="24" t="s">
+        <v>815</v>
+      </c>
+      <c r="D2" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="20" t="s">
-        <v>740</v>
+      <c r="E2" s="19" t="s">
+        <v>737</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="17">
-        <f t="shared" ref="A3:A34" si="0">A2+1</f>
+      <c r="A3" s="28">
+        <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>718</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>103</v>
+      <c r="D3" s="19" t="s">
+        <v>86</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="17">
-        <f t="shared" si="0"/>
+      <c r="A4" s="28">
+        <f>A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>718</v>
       </c>
-      <c r="D4" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="E4" s="22" t="s">
-        <v>688</v>
+      <c r="D4" s="19" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="17">
-        <f t="shared" si="0"/>
+      <c r="A5" s="28">
+        <f>A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>728</v>
-      </c>
-      <c r="D5" s="20" t="s">
+        <v>727</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="28">
+        <f>A5+1</f>
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="D6" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E6" s="19" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="28">
+        <f>A6+1</f>
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>697</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="28">
+        <f>A7+1</f>
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>696</v>
+      </c>
+      <c r="E8" s="19" t="s">
         <v>741</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="17">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>728</v>
-      </c>
-      <c r="D6" s="20" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="28">
+        <f>A8+1</f>
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="D9" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="20" t="s">
-        <v>819</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="17">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>728</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="17">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>728</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>696</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>744</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="17">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>728</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>697</v>
-      </c>
-      <c r="E9" s="24" t="s">
-        <v>745</v>
+      <c r="E9" s="19" t="s">
+        <v>808</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="17">
-        <f t="shared" si="0"/>
+      <c r="A10" s="28">
+        <f>A9+1</f>
         <v>9</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>735</v>
-      </c>
-      <c r="D10" s="7" t="s">
+        <v>734</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="28">
+        <f>A10+1</f>
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>734</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>695</v>
       </c>
-      <c r="E10" s="23" t="s">
-        <v>743</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="17">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>735</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>746</v>
+      <c r="E11" s="22" t="s">
+        <v>740</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="17">
-        <f t="shared" si="0"/>
+      <c r="A12" s="28">
+        <f>A11+1</f>
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>719</v>
       </c>
-      <c r="D12" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>747</v>
+      <c r="D12" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>745</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="17">
-        <f t="shared" si="0"/>
+      <c r="A13" s="28">
+        <f>A12+1</f>
         <v>12</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>719</v>
       </c>
-      <c r="D13" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>748</v>
+      <c r="D13" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>809</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="17">
-        <f t="shared" si="0"/>
+      <c r="A14" s="28">
+        <f>A13+1</f>
         <v>13</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>719</v>
       </c>
-      <c r="D14" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>128</v>
+      <c r="D14" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>744</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="17">
-        <f t="shared" si="0"/>
+      <c r="A15" s="28">
+        <f>A14+1</f>
         <v>14</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>719</v>
       </c>
-      <c r="D15" s="20" t="s">
-        <v>83</v>
+      <c r="D15" s="19" t="s">
+        <v>6</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>749</v>
+        <v>746</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="17">
-        <f t="shared" si="0"/>
+      <c r="A16" s="28">
+        <f>A15+1</f>
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>719</v>
       </c>
-      <c r="D16" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="21" t="s">
-        <v>750</v>
+      <c r="D16" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="17">
-        <f t="shared" si="0"/>
+      <c r="A17" s="28">
+        <f>A16+1</f>
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>729</v>
-      </c>
-      <c r="D17" s="20" t="s">
+        <v>728</v>
+      </c>
+      <c r="D17" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="19" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="17">
-        <f t="shared" si="0"/>
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="28">
+        <f>A17+1</f>
         <v>17</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="25" t="s">
         <v>712</v>
       </c>
-      <c r="D18" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>751</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="17">
-        <f t="shared" si="0"/>
+      <c r="C18" s="29" t="s">
+        <v>785</v>
+      </c>
+      <c r="D18" s="33" t="s">
+        <v>788</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="28">
+        <f>A18+1</f>
         <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>712</v>
       </c>
-      <c r="D19" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="20" t="s">
-        <v>752</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="17">
-        <f t="shared" si="0"/>
+      <c r="D19" s="19" t="s">
+        <v>731</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="28">
+        <f>A19+1</f>
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>712</v>
       </c>
-      <c r="D20" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="17">
-        <f t="shared" si="0"/>
+      <c r="D20" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>747</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="28">
+        <f>A20+1</f>
         <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>712</v>
       </c>
-      <c r="D21" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="17">
-        <f t="shared" si="0"/>
+      <c r="D21" s="19" t="s">
+        <v>723</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="28">
+        <f>A21+1</f>
         <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>712</v>
       </c>
-      <c r="D22" s="20" t="s">
-        <v>80</v>
+      <c r="D22" s="19" t="s">
+        <v>4</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="17">
-        <f t="shared" si="0"/>
+        <v>810</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="28">
+        <f>A22+1</f>
         <v>22</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="25" t="s">
         <v>712</v>
       </c>
-      <c r="D23" s="20" t="s">
-        <v>705</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="17">
-        <f t="shared" si="0"/>
+      <c r="C23" s="29" t="s">
+        <v>790</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>791</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="28">
+        <f>A23+1</f>
         <v>23</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>712</v>
       </c>
-      <c r="D24" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>753</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="17">
-        <f t="shared" si="0"/>
+      <c r="D24" s="19" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="28">
+        <f>A24+1</f>
         <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>712</v>
       </c>
-      <c r="D25" s="20" t="s">
-        <v>93</v>
+      <c r="D25" s="19" t="s">
+        <v>96</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="17">
-        <f t="shared" si="0"/>
+        <v>748</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A26" s="28">
+        <f>A25+1</f>
         <v>25</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>712</v>
       </c>
-      <c r="D26" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="E26" s="21" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="17">
-        <f t="shared" si="0"/>
+      <c r="D26" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="28">
+        <f>A26+1</f>
         <v>26</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="25" t="s">
         <v>712</v>
       </c>
-      <c r="D27" s="20" t="s">
-        <v>723</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>755</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="17">
-        <f t="shared" si="0"/>
+      <c r="C27" s="29" t="s">
+        <v>778</v>
+      </c>
+      <c r="D27" s="29" t="s">
+        <v>779</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>806</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="28">
+        <f>A27+1</f>
         <v>27</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>712</v>
       </c>
-      <c r="D28" s="20" t="s">
+      <c r="D28" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="28">
+        <f>A28+1</f>
+        <v>28</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="C29" s="29" t="s">
+        <v>785</v>
+      </c>
+      <c r="D29" s="29" t="s">
+        <v>786</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A30" s="28">
+        <f>A29+1</f>
+        <v>29</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>785</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>789</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A31" s="28">
+        <f>A30+1</f>
+        <v>30</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>712</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>705</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="28">
+        <f>A31+1</f>
+        <v>31</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>712</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="28">
+        <f>A32+1</f>
+        <v>32</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>781</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>782</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="28">
+        <f>A33+1</f>
+        <v>33</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>774</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>776</v>
+      </c>
+      <c r="E34" s="30" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A35" s="28">
+        <f>A34+1</f>
+        <v>34</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="C35" s="29" t="s">
+        <v>764</v>
+      </c>
+      <c r="D35" s="29" t="s">
+        <v>657</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36" s="28">
+        <f>A35+1</f>
+        <v>35</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="C36" s="29" t="s">
+        <v>774</v>
+      </c>
+      <c r="D36" s="29" t="s">
+        <v>777</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A37" s="28">
+        <f>A36+1</f>
+        <v>36</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>778</v>
+      </c>
+      <c r="D37" s="29" t="s">
+        <v>780</v>
+      </c>
+      <c r="E37" s="30" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="28">
+        <f>A37+1</f>
+        <v>37</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="C38" s="29" t="s">
+        <v>785</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>787</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="28">
+        <f>A38+1</f>
+        <v>38</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="C39" s="29" t="s">
+        <v>783</v>
+      </c>
+      <c r="D39" s="29" t="s">
+        <v>784</v>
+      </c>
+      <c r="E39" s="30" t="s">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="28">
+        <f>A39+1</f>
+        <v>39</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="C40" s="29" t="s">
+        <v>765</v>
+      </c>
+      <c r="D40" s="29" t="s">
+        <v>768</v>
+      </c>
+      <c r="E40" s="31" t="s">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="28">
+        <f>A40+1</f>
+        <v>40</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="C41" s="29" t="s">
+        <v>765</v>
+      </c>
+      <c r="D41" s="29" t="s">
+        <v>770</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="28">
+        <f>A41+1</f>
+        <v>41</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="C42" s="29" t="s">
+        <v>765</v>
+      </c>
+      <c r="D42" s="29" t="s">
+        <v>766</v>
+      </c>
+      <c r="E42" s="31" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="28">
+        <f>A42+1</f>
+        <v>42</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="C43" s="29" t="s">
+        <v>772</v>
+      </c>
+      <c r="D43" s="29" t="s">
+        <v>773</v>
+      </c>
+      <c r="E43" s="30" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="28">
+        <f>A43+1</f>
+        <v>43</v>
+      </c>
+      <c r="B44" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="C44" s="29" t="s">
+        <v>765</v>
+      </c>
+      <c r="D44" s="29" t="s">
+        <v>767</v>
+      </c>
+      <c r="E44" s="31" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A45" s="28">
+        <f>A44+1</f>
+        <v>44</v>
+      </c>
+      <c r="B45" s="25" t="s">
+        <v>712</v>
+      </c>
+      <c r="C45" s="29" t="s">
+        <v>774</v>
+      </c>
+      <c r="D45" s="29" t="s">
+        <v>775</v>
+      </c>
+      <c r="E45" s="30" t="s">
+        <v>804</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="28">
+        <f>A45+1</f>
+        <v>45</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>712</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A47" s="28">
+        <f>A46+1</f>
+        <v>46</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>712</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>729</v>
+      </c>
+      <c r="E47" s="19" t="s">
         <v>730</v>
       </c>
-      <c r="E28" s="20" t="s">
-        <v>731</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="17">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>712</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>732</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>733</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="17">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B30" s="26" t="s">
-        <v>712</v>
-      </c>
-      <c r="C30" s="27" t="s">
-        <v>772</v>
-      </c>
-      <c r="D30" s="27" t="s">
-        <v>657</v>
-      </c>
-      <c r="E30" s="28" t="s">
-        <v>813</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="17">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B31" s="26" t="s">
-        <v>712</v>
-      </c>
-      <c r="C31" s="27" t="s">
-        <v>773</v>
-      </c>
-      <c r="D31" s="27" t="s">
-        <v>774</v>
-      </c>
-      <c r="E31" s="30" t="s">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="17">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B32" s="26" t="s">
-        <v>712</v>
-      </c>
-      <c r="C32" s="27" t="s">
-        <v>773</v>
-      </c>
-      <c r="D32" s="27" t="s">
-        <v>775</v>
-      </c>
-      <c r="E32" s="30" t="s">
-        <v>814</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="17">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B33" s="26" t="s">
-        <v>712</v>
-      </c>
-      <c r="C33" s="27" t="s">
-        <v>773</v>
-      </c>
-      <c r="D33" s="27" t="s">
-        <v>776</v>
-      </c>
-      <c r="E33" s="30" t="s">
-        <v>777</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="17">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B34" s="26" t="s">
-        <v>712</v>
-      </c>
-      <c r="C34" s="27" t="s">
-        <v>773</v>
-      </c>
-      <c r="D34" s="27" t="s">
-        <v>778</v>
-      </c>
-      <c r="E34" s="30" t="s">
-        <v>779</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="17">
-        <f t="shared" ref="A35:A66" si="1">A34+1</f>
-        <v>34</v>
-      </c>
-      <c r="B35" s="26" t="s">
-        <v>712</v>
-      </c>
-      <c r="C35" s="27" t="s">
-        <v>780</v>
-      </c>
-      <c r="D35" s="27" t="s">
-        <v>781</v>
-      </c>
-      <c r="E35" s="28" t="s">
-        <v>801</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="17">
-        <f t="shared" si="1"/>
-        <v>35</v>
-      </c>
-      <c r="B36" s="26" t="s">
-        <v>712</v>
-      </c>
-      <c r="C36" s="27" t="s">
-        <v>782</v>
-      </c>
-      <c r="D36" s="27" t="s">
-        <v>783</v>
-      </c>
-      <c r="E36" s="28" t="s">
-        <v>815</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="17">
-        <f t="shared" si="1"/>
-        <v>36</v>
-      </c>
-      <c r="B37" s="26" t="s">
-        <v>712</v>
-      </c>
-      <c r="C37" s="27" t="s">
-        <v>782</v>
-      </c>
-      <c r="D37" s="27" t="s">
-        <v>784</v>
-      </c>
-      <c r="E37" s="28" t="s">
-        <v>816</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" s="17">
-        <f t="shared" si="1"/>
-        <v>37</v>
-      </c>
-      <c r="B38" s="26" t="s">
-        <v>712</v>
-      </c>
-      <c r="C38" s="27" t="s">
-        <v>782</v>
-      </c>
-      <c r="D38" s="27" t="s">
-        <v>785</v>
-      </c>
-      <c r="E38" s="28" t="s">
-        <v>802</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="17">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="B39" s="26" t="s">
-        <v>712</v>
-      </c>
-      <c r="C39" s="27" t="s">
-        <v>786</v>
-      </c>
-      <c r="D39" s="27" t="s">
-        <v>787</v>
-      </c>
-      <c r="E39" s="28" t="s">
-        <v>817</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="17">
-        <f t="shared" si="1"/>
-        <v>39</v>
-      </c>
-      <c r="B40" s="26" t="s">
-        <v>712</v>
-      </c>
-      <c r="C40" s="27" t="s">
-        <v>786</v>
-      </c>
-      <c r="D40" s="27" t="s">
-        <v>788</v>
-      </c>
-      <c r="E40" s="28" t="s">
-        <v>812</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="17">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="B41" s="26" t="s">
-        <v>712</v>
-      </c>
-      <c r="C41" s="27" t="s">
-        <v>789</v>
-      </c>
-      <c r="D41" s="27" t="s">
-        <v>790</v>
-      </c>
-      <c r="E41" s="29" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="17">
-        <f t="shared" si="1"/>
-        <v>41</v>
-      </c>
-      <c r="B42" s="26" t="s">
-        <v>712</v>
-      </c>
-      <c r="C42" s="27" t="s">
-        <v>791</v>
-      </c>
-      <c r="D42" s="27" t="s">
-        <v>792</v>
-      </c>
-      <c r="E42" s="28" t="s">
-        <v>804</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="17">
-        <f t="shared" si="1"/>
-        <v>42</v>
-      </c>
-      <c r="B43" s="26" t="s">
-        <v>712</v>
-      </c>
-      <c r="C43" s="27" t="s">
-        <v>793</v>
-      </c>
-      <c r="D43" s="27" t="s">
-        <v>794</v>
-      </c>
-      <c r="E43" s="28" t="s">
-        <v>805</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="17">
-        <f t="shared" si="1"/>
-        <v>43</v>
-      </c>
-      <c r="B44" s="26" t="s">
-        <v>712</v>
-      </c>
-      <c r="C44" s="27" t="s">
-        <v>793</v>
-      </c>
-      <c r="D44" s="27" t="s">
-        <v>795</v>
-      </c>
-      <c r="E44" s="28" t="s">
-        <v>806</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="17">
-        <f t="shared" si="1"/>
-        <v>44</v>
-      </c>
-      <c r="B45" s="26" t="s">
-        <v>712</v>
-      </c>
-      <c r="C45" s="27" t="s">
-        <v>793</v>
-      </c>
-      <c r="D45" s="31" t="s">
-        <v>796</v>
-      </c>
-      <c r="E45" s="28" t="s">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="17">
-        <f t="shared" si="1"/>
-        <v>45</v>
-      </c>
-      <c r="B46" s="26" t="s">
-        <v>712</v>
-      </c>
-      <c r="C46" s="27" t="s">
-        <v>793</v>
-      </c>
-      <c r="D46" s="27" t="s">
-        <v>797</v>
-      </c>
-      <c r="E46" s="28" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="17">
-        <f t="shared" si="1"/>
-        <v>46</v>
-      </c>
-      <c r="B47" s="26" t="s">
-        <v>712</v>
-      </c>
-      <c r="C47" s="27" t="s">
-        <v>798</v>
-      </c>
-      <c r="D47" s="27" t="s">
-        <v>799</v>
-      </c>
-      <c r="E47" s="28" t="s">
-        <v>809</v>
-      </c>
     </row>
     <row r="48" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A48" s="17">
-        <f t="shared" si="1"/>
+      <c r="A48" s="28">
+        <f>A47+1</f>
         <v>47</v>
       </c>
       <c r="B48" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D48" s="20" t="s">
-        <v>0</v>
-      </c>
-      <c r="E48" s="21" t="s">
-        <v>756</v>
+      <c r="D48" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="E48" s="20" t="s">
+        <v>661</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A49" s="17">
-        <f t="shared" si="1"/>
+      <c r="A49" s="28">
+        <f>A48+1</f>
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D49" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E49" s="21" t="s">
-        <v>757</v>
+      <c r="D49" s="19" t="s">
+        <v>722</v>
+      </c>
+      <c r="E49" s="19" t="s">
+        <v>755</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A50" s="17">
-        <f t="shared" si="1"/>
+      <c r="A50" s="28">
+        <f>A49+1</f>
         <v>49</v>
       </c>
       <c r="B50" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D50" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E50" s="21" t="s">
-        <v>661</v>
+      <c r="D50" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E50" s="20" t="s">
+        <v>751</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A51" s="17">
-        <f t="shared" si="1"/>
+      <c r="A51" s="28">
+        <f>A50+1</f>
         <v>50</v>
       </c>
       <c r="B51" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D51" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="E51" s="21" t="s">
-        <v>758</v>
+      <c r="D51" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E51" s="20" t="s">
+        <v>753</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A52" s="17">
-        <f t="shared" si="1"/>
+      <c r="A52" s="28">
+        <f>A51+1</f>
         <v>51</v>
       </c>
       <c r="B52" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D52" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="E52" s="21" t="s">
-        <v>739</v>
+      <c r="D52" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E52" s="19" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A53" s="17">
-        <f t="shared" si="1"/>
+      <c r="A53" s="28">
+        <f>A52+1</f>
         <v>52</v>
       </c>
       <c r="B53" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D53" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="21" t="s">
-        <v>759</v>
+      <c r="D53" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="E53" s="20" t="s">
+        <v>813</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A54" s="17">
-        <f t="shared" si="1"/>
+      <c r="A54" s="28">
+        <f>A53+1</f>
         <v>53</v>
       </c>
       <c r="B54" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D54" s="20" t="s">
-        <v>69</v>
+      <c r="D54" s="19" t="s">
+        <v>3</v>
       </c>
       <c r="E54" s="20" t="s">
-        <v>760</v>
+        <v>752</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A55" s="17">
-        <f t="shared" si="1"/>
+      <c r="A55" s="28">
+        <f>A54+1</f>
         <v>54</v>
       </c>
       <c r="B55" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D55" s="20" t="s">
-        <v>722</v>
+      <c r="D55" s="19" t="s">
+        <v>0</v>
       </c>
       <c r="E55" s="20" t="s">
-        <v>761</v>
+        <v>750</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="17">
-        <f t="shared" si="1"/>
+      <c r="A56" s="28">
+        <f>A55+1</f>
         <v>55</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>713</v>
       </c>
-      <c r="D56" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="E56" s="21" t="s">
-        <v>762</v>
+      <c r="D56" s="19" t="s">
+        <v>720</v>
+      </c>
+      <c r="E56" s="19" t="s">
+        <v>807</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="17">
-        <f t="shared" si="1"/>
+      <c r="A57" s="28">
+        <f>A56+1</f>
         <v>56</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>713</v>
       </c>
-      <c r="D57" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="E57" s="21" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="17">
-        <f t="shared" si="1"/>
+      <c r="D57" s="19" t="s">
+        <v>724</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>757</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="28">
+        <f>A57+1</f>
         <v>57</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>713</v>
       </c>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="E58" s="21" t="s">
-        <v>721</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="17">
-        <f t="shared" si="1"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E58" s="20" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="28">
+        <f>A58+1</f>
         <v>58</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>713</v>
       </c>
-      <c r="C59" s="20"/>
-      <c r="D59" s="20" t="s">
-        <v>706</v>
-      </c>
-      <c r="E59" s="22" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="17">
-        <f t="shared" si="1"/>
+      <c r="C59" s="19"/>
+      <c r="D59" s="19" t="s">
+        <v>726</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="28">
+        <f>A59+1</f>
         <v>59</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>713</v>
       </c>
-      <c r="C60" s="20"/>
-      <c r="D60" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="E60" s="21" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="17">
-        <f t="shared" si="1"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19" t="s">
+        <v>725</v>
+      </c>
+      <c r="E60" s="19" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="28">
+        <f>A60+1</f>
         <v>60</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>713</v>
       </c>
-      <c r="C61" s="20"/>
-      <c r="D61" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="E61" s="21" t="s">
-        <v>686</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="17">
-        <f t="shared" si="1"/>
+      <c r="C61" s="19"/>
+      <c r="D61" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="E61" s="20" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="28">
+        <f>A61+1</f>
         <v>61</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>713</v>
       </c>
-      <c r="C62" s="20"/>
-      <c r="D62" s="20" t="s">
-        <v>720</v>
+      <c r="C62" s="19"/>
+      <c r="D62" s="19" t="s">
+        <v>99</v>
       </c>
       <c r="E62" s="20" t="s">
-        <v>818</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="17">
-        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="28">
+        <f>A62+1</f>
         <v>62</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>713</v>
       </c>
-      <c r="C63" s="20"/>
-      <c r="D63" s="20" t="s">
-        <v>724</v>
+      <c r="C63" s="19"/>
+      <c r="D63" s="19" t="s">
+        <v>97</v>
       </c>
       <c r="E63" s="20" t="s">
-        <v>763</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="17">
-        <f t="shared" si="1"/>
+        <v>756</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="28">
+        <f>A63+1</f>
         <v>63</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>713</v>
       </c>
-      <c r="C64" s="20"/>
-      <c r="D64" s="20" t="s">
-        <v>725</v>
+      <c r="C64" s="19"/>
+      <c r="D64" s="19" t="s">
+        <v>98</v>
       </c>
       <c r="E64" s="20" t="s">
-        <v>738</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="17">
-        <f t="shared" si="1"/>
+        <v>721</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="28">
+        <f>A64+1</f>
         <v>64</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>713</v>
       </c>
-      <c r="C65" s="20"/>
-      <c r="D65" s="20" t="s">
-        <v>726</v>
-      </c>
-      <c r="E65" s="20" t="s">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="17">
-        <f t="shared" si="1"/>
+      <c r="C65" s="19"/>
+      <c r="D65" s="19" t="s">
+        <v>706</v>
+      </c>
+      <c r="E65" s="21" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="28">
+        <f>A65+1</f>
         <v>65</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>714</v>
       </c>
-      <c r="C66" s="20"/>
-      <c r="D66" s="20" t="s">
-        <v>811</v>
+      <c r="C66" s="19"/>
+      <c r="D66" s="19" t="s">
+        <v>678</v>
       </c>
       <c r="E66" s="20" t="s">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="17">
-        <f t="shared" ref="A67:A75" si="2">A66+1</f>
+        <v>761</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="28">
+        <f>A66+1</f>
         <v>66</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>714</v>
       </c>
-      <c r="C67" s="20"/>
-      <c r="D67" s="20" t="s">
+      <c r="C67" s="19"/>
+      <c r="D67" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="E67" s="21" t="s">
-        <v>766</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="17">
-        <f t="shared" si="2"/>
+      <c r="E67" s="20" t="s">
+        <v>760</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="28">
+        <f>A67+1</f>
         <v>67</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>714</v>
       </c>
-      <c r="C68" s="20"/>
-      <c r="D68" s="20" t="s">
-        <v>678</v>
-      </c>
-      <c r="E68" s="21" t="s">
-        <v>767</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="17">
-        <f t="shared" si="2"/>
+      <c r="C68" s="19"/>
+      <c r="D68" s="19" t="s">
+        <v>800</v>
+      </c>
+      <c r="E68" s="19" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="28">
+        <f>A68+1</f>
         <v>68</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>714</v>
       </c>
-      <c r="C69" s="20"/>
-      <c r="D69" s="20" t="s">
+      <c r="C69" s="19"/>
+      <c r="D69" s="19" t="s">
         <v>679</v>
       </c>
-      <c r="E69" s="23" t="s">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="17">
-        <f t="shared" si="2"/>
+      <c r="E69" s="22" t="s">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="28">
+        <f>A69+1</f>
         <v>69</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>734</v>
-      </c>
-      <c r="C70" s="20"/>
-      <c r="D70" s="20" t="s">
+        <v>733</v>
+      </c>
+      <c r="C70" s="19"/>
+      <c r="D70" s="19" t="s">
+        <v>799</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="28">
+        <f>A70+1</f>
+        <v>70</v>
+      </c>
+      <c r="B71" s="6" t="s">
+        <v>733</v>
+      </c>
+      <c r="C71" s="19"/>
+      <c r="D71" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E70" s="20" t="s">
-        <v>769</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="17">
-        <f t="shared" si="2"/>
-        <v>70</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>734</v>
-      </c>
-      <c r="C71" s="20"/>
-      <c r="D71" s="20" t="s">
-        <v>810</v>
-      </c>
-      <c r="E71" s="20" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="17">
-        <f t="shared" si="2"/>
+      <c r="E71" s="19" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="28">
+        <f>A71+1</f>
         <v>71</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>715</v>
       </c>
-      <c r="C72" s="20"/>
-      <c r="D72" s="20" t="s">
+      <c r="C72" s="19"/>
+      <c r="D72" s="19" t="s">
         <v>709</v>
       </c>
-      <c r="E72" s="20" t="s">
-        <v>770</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="17">
-        <f t="shared" si="2"/>
+      <c r="E72" s="19" t="s">
+        <v>814</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="28">
+        <f>A72+1</f>
         <v>72</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>717</v>
       </c>
-      <c r="C73" s="20"/>
-      <c r="D73" s="20" t="s">
+      <c r="C73" s="19"/>
+      <c r="D73" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="E73" s="22" t="s">
-        <v>771</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="17">
-        <f t="shared" si="2"/>
+      <c r="E73" s="21" t="s">
+        <v>763</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="28">
+        <f>A73+1</f>
         <v>73</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>717</v>
       </c>
-      <c r="C74" s="20"/>
-      <c r="D74" s="20" t="s">
+      <c r="C74" s="19"/>
+      <c r="D74" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="E74" s="21" t="s">
+      <c r="E74" s="20" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="75" spans="1:5" s="29" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="17">
-        <f t="shared" si="2"/>
+    <row r="75" spans="1:5" s="32" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="28">
+        <f>A74+1</f>
         <v>74</v>
       </c>
       <c r="B75" s="6" t="s">
         <v>716</v>
       </c>
-      <c r="C75" s="20"/>
-      <c r="D75" s="20" t="s">
+      <c r="C75" s="19"/>
+      <c r="D75" s="19" t="s">
         <v>700</v>
       </c>
-      <c r="E75" s="20" t="s">
-        <v>737</v>
+      <c r="E75" s="19" t="s">
+        <v>735</v>
       </c>
     </row>
   </sheetData>
@@ -7535,7 +7536,7 @@
       <c r="A25" s="15" t="s">
         <v>698</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="17" t="s">
         <v>699</v>
       </c>
     </row>
@@ -7543,7 +7544,7 @@
       <c r="A26" s="15" t="s">
         <v>702</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="17" t="s">
         <v>704</v>
       </c>
     </row>
@@ -7551,15 +7552,15 @@
       <c r="A27" s="15" t="s">
         <v>703</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="17" t="s">
         <v>708</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="18" t="s">
         <v>710</v>
       </c>
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="17" t="s">
         <v>711</v>
       </c>
     </row>
@@ -7706,7 +7707,7 @@
       <c r="A17" s="10"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="32" t="s">
+      <c r="A18" s="26" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="10" t="s">
@@ -7714,25 +7715,25 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="32"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="10" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="32"/>
+      <c r="A20" s="26"/>
       <c r="B20" s="11" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="32"/>
+      <c r="A21" s="26"/>
       <c r="B21" s="10" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="32" t="s">
+      <c r="A22" s="26" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="10" t="s">
@@ -7740,13 +7741,13 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="32"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="10" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="32" t="s">
+      <c r="A24" s="26" t="s">
         <v>154</v>
       </c>
       <c r="B24" s="10" t="s">
@@ -7754,7 +7755,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="32"/>
+      <c r="A25" s="26"/>
       <c r="B25" s="10" t="s">
         <v>156</v>
       </c>
@@ -7795,7 +7796,7 @@
       <c r="A30" s="10"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="33" t="s">
+      <c r="A31" s="27" t="s">
         <v>157</v>
       </c>
       <c r="B31" s="10" t="s">
@@ -7803,7 +7804,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="33"/>
+      <c r="A32" s="27"/>
       <c r="B32" s="10" t="s">
         <v>162</v>
       </c>
@@ -7856,7 +7857,7 @@
       <c r="A42" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="B42" s="33" t="s">
+      <c r="B42" s="27" t="s">
         <v>174</v>
       </c>
     </row>
@@ -7864,13 +7865,13 @@
       <c r="A43" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="B43" s="33"/>
+      <c r="B43" s="27"/>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="B44" s="33"/>
+      <c r="B44" s="27"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="10"/>
@@ -7903,7 +7904,7 @@
       <c r="A49" s="10"/>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50" s="32" t="s">
+      <c r="A50" s="26" t="s">
         <v>157</v>
       </c>
       <c r="B50" s="11" t="s">
@@ -7911,37 +7912,37 @@
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51" s="32"/>
+      <c r="A51" s="26"/>
       <c r="B51" s="10" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52" s="32"/>
+      <c r="A52" s="26"/>
       <c r="B52" s="10" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53" s="32"/>
+      <c r="A53" s="26"/>
       <c r="B53" s="10" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54" s="32"/>
+      <c r="A54" s="26"/>
       <c r="B54" s="10" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55" s="32"/>
+      <c r="A55" s="26"/>
       <c r="B55" s="10" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56" s="32"/>
+      <c r="A56" s="26"/>
       <c r="B56" s="10" t="s">
         <v>186</v>
       </c>
@@ -7957,7 +7958,7 @@
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A59" s="32" t="s">
+      <c r="A59" s="26" t="s">
         <v>150</v>
       </c>
       <c r="B59" s="10" t="s">
@@ -7965,10 +7966,10 @@
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A60" s="32"/>
+      <c r="A60" s="26"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A61" s="32"/>
+      <c r="A61" s="26"/>
       <c r="B61" s="10" t="s">
         <v>190</v>
       </c>
@@ -8018,7 +8019,7 @@
       <c r="A69" s="10"/>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A70" s="32" t="s">
+      <c r="A70" s="26" t="s">
         <v>157</v>
       </c>
       <c r="B70" s="10" t="s">
@@ -8026,19 +8027,19 @@
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A71" s="32"/>
+      <c r="A71" s="26"/>
       <c r="B71" s="11" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A72" s="32"/>
+      <c r="A72" s="26"/>
       <c r="B72" s="10" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A73" s="32"/>
+      <c r="A73" s="26"/>
       <c r="B73" s="10" t="s">
         <v>200</v>
       </c>
@@ -8183,7 +8184,7 @@
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A97" s="32" t="s">
+      <c r="A97" s="26" t="s">
         <v>222</v>
       </c>
       <c r="B97" s="10" t="s">
@@ -8191,19 +8192,19 @@
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A98" s="32"/>
+      <c r="A98" s="26"/>
       <c r="B98" s="11" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A99" s="32"/>
+      <c r="A99" s="26"/>
       <c r="B99" s="10" t="s">
         <v>224</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A100" s="32"/>
+      <c r="A100" s="26"/>
       <c r="B100" s="10" t="s">
         <v>225</v>
       </c>
@@ -8268,7 +8269,7 @@
       <c r="A111" s="10"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A112" s="32" t="s">
+      <c r="A112" s="26" t="s">
         <v>150</v>
       </c>
       <c r="B112" s="10" t="s">
@@ -8276,7 +8277,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113" s="32"/>
+      <c r="A113" s="26"/>
       <c r="B113" s="10" t="s">
         <v>233</v>
       </c>
@@ -8285,7 +8286,7 @@
       <c r="A114" s="10"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A115" s="32" t="s">
+      <c r="A115" s="26" t="s">
         <v>157</v>
       </c>
       <c r="B115" s="10" t="s">
@@ -8293,19 +8294,19 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" s="32"/>
+      <c r="A116" s="26"/>
       <c r="B116" s="10" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" s="32"/>
+      <c r="A117" s="26"/>
       <c r="B117" s="10" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A118" s="32"/>
+      <c r="A118" s="26"/>
       <c r="B118" s="10" t="s">
         <v>237</v>
       </c>
@@ -8333,61 +8334,61 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A123" s="32" t="s">
+      <c r="A123" s="26" t="s">
         <v>241</v>
       </c>
       <c r="B123" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="C123" s="33" t="s">
+      <c r="C123" s="27" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A124" s="32"/>
+      <c r="A124" s="26"/>
       <c r="B124" s="12" t="s">
         <v>243</v>
       </c>
-      <c r="C124" s="33"/>
+      <c r="C124" s="27"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A125" s="32" t="s">
+      <c r="A125" s="26" t="s">
         <v>245</v>
       </c>
       <c r="B125" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="C125" s="33" t="s">
+      <c r="C125" s="27" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A126" s="32"/>
+      <c r="A126" s="26"/>
       <c r="B126" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="C126" s="33"/>
+      <c r="C126" s="27"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A127" s="32" t="s">
+      <c r="A127" s="26" t="s">
         <v>249</v>
       </c>
       <c r="B127" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="C127" s="33" t="s">
+      <c r="C127" s="27" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A128" s="32"/>
+      <c r="A128" s="26"/>
       <c r="B128" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="C128" s="33"/>
+      <c r="C128" s="27"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A129" s="32" t="s">
+      <c r="A129" s="26" t="s">
         <v>253</v>
       </c>
       <c r="B129" s="10" t="s">
@@ -8398,7 +8399,7 @@
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A130" s="32"/>
+      <c r="A130" s="26"/>
       <c r="B130" s="10" t="s">
         <v>255</v>
       </c>
@@ -8407,7 +8408,7 @@
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A131" s="32"/>
+      <c r="A131" s="26"/>
       <c r="B131" s="10" t="s">
         <v>256</v>
       </c>
@@ -8416,7 +8417,7 @@
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A132" s="32"/>
+      <c r="A132" s="26"/>
       <c r="B132" s="10" t="s">
         <v>257</v>
       </c>
@@ -8425,7 +8426,7 @@
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A133" s="32"/>
+      <c r="A133" s="26"/>
       <c r="B133" s="10" t="s">
         <v>258</v>
       </c>
@@ -8434,7 +8435,7 @@
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A134" s="32"/>
+      <c r="A134" s="26"/>
       <c r="B134" s="10" t="s">
         <v>259</v>
       </c>
@@ -8443,17 +8444,17 @@
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A135" s="32"/>
+      <c r="A135" s="26"/>
       <c r="B135" s="10"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A136" s="32"/>
+      <c r="A136" s="26"/>
       <c r="B136" s="10" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A137" s="32" t="s">
+      <c r="A137" s="26" t="s">
         <v>267</v>
       </c>
       <c r="B137" s="10" t="s">
@@ -8464,7 +8465,7 @@
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A138" s="32"/>
+      <c r="A138" s="26"/>
       <c r="B138" s="10" t="s">
         <v>269</v>
       </c>
@@ -8473,7 +8474,7 @@
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A139" s="32" t="s">
+      <c r="A139" s="26" t="s">
         <v>272</v>
       </c>
       <c r="B139" s="10" t="s">
@@ -8484,7 +8485,7 @@
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A140" s="32"/>
+      <c r="A140" s="26"/>
       <c r="B140" s="10" t="s">
         <v>274</v>
       </c>
@@ -8493,7 +8494,7 @@
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A141" s="32" t="s">
+      <c r="A141" s="26" t="s">
         <v>277</v>
       </c>
       <c r="B141" s="10" t="s">
@@ -8504,7 +8505,7 @@
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A142" s="32"/>
+      <c r="A142" s="26"/>
       <c r="B142" s="10" t="s">
         <v>279</v>
       </c>
@@ -8513,7 +8514,7 @@
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A143" s="32" t="s">
+      <c r="A143" s="26" t="s">
         <v>282</v>
       </c>
       <c r="B143" s="10" t="s">
@@ -8524,7 +8525,7 @@
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A144" s="32"/>
+      <c r="A144" s="26"/>
       <c r="B144" s="10" t="s">
         <v>284</v>
       </c>
@@ -8533,31 +8534,31 @@
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A145" s="32"/>
+      <c r="A145" s="26"/>
       <c r="C145" s="10" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A146" s="32" t="s">
+      <c r="A146" s="26" t="s">
         <v>288</v>
       </c>
       <c r="B146" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="C146" s="33" t="s">
+      <c r="C146" s="27" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A147" s="32"/>
+      <c r="A147" s="26"/>
       <c r="B147" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="C147" s="33"/>
+      <c r="C147" s="27"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A148" s="32" t="s">
+      <c r="A148" s="26" t="s">
         <v>292</v>
       </c>
       <c r="B148" s="10" t="s">
@@ -8568,7 +8569,7 @@
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A149" s="32"/>
+      <c r="A149" s="26"/>
       <c r="B149" s="10" t="s">
         <v>294</v>
       </c>
@@ -8577,14 +8578,14 @@
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A150" s="32"/>
+      <c r="A150" s="26"/>
       <c r="B150" s="10"/>
       <c r="C150" s="10" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A151" s="32"/>
+      <c r="A151" s="26"/>
       <c r="B151" s="10" t="s">
         <v>295</v>
       </c>
@@ -8593,14 +8594,14 @@
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A152" s="32"/>
+      <c r="A152" s="26"/>
       <c r="B152" s="10"/>
       <c r="C152" s="10" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A153" s="32"/>
+      <c r="A153" s="26"/>
       <c r="B153" s="10" t="s">
         <v>296</v>
       </c>
@@ -8609,7 +8610,7 @@
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A154" s="32"/>
+      <c r="A154" s="26"/>
       <c r="B154" s="10" t="s">
         <v>297</v>
       </c>
@@ -8618,7 +8619,7 @@
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A155" s="32"/>
+      <c r="A155" s="26"/>
       <c r="B155" s="10" t="s">
         <v>298</v>
       </c>
@@ -8627,7 +8628,7 @@
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A156" s="32"/>
+      <c r="A156" s="26"/>
       <c r="B156" s="10" t="s">
         <v>299</v>
       </c>
@@ -8636,29 +8637,29 @@
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A157" s="32"/>
+      <c r="A157" s="26"/>
       <c r="B157" s="10" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A158" s="32"/>
+      <c r="A158" s="26"/>
       <c r="B158" s="10"/>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A159" s="32"/>
+      <c r="A159" s="26"/>
       <c r="B159" s="11" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A160" s="32"/>
+      <c r="A160" s="26"/>
       <c r="B160" s="10" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A161" s="32" t="s">
+      <c r="A161" s="26" t="s">
         <v>311</v>
       </c>
       <c r="B161" s="10" t="s">
@@ -8669,7 +8670,7 @@
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A162" s="32"/>
+      <c r="A162" s="26"/>
       <c r="B162" s="10" t="s">
         <v>313</v>
       </c>
@@ -8678,7 +8679,7 @@
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A163" s="32"/>
+      <c r="A163" s="26"/>
       <c r="B163" s="10" t="s">
         <v>296</v>
       </c>
@@ -8687,16 +8688,16 @@
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A164" s="32"/>
+      <c r="A164" s="26"/>
       <c r="B164" s="10" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A165" s="32" t="s">
+      <c r="A165" s="26" t="s">
         <v>317</v>
       </c>
-      <c r="B165" s="33" t="s">
+      <c r="B165" s="27" t="s">
         <v>318</v>
       </c>
       <c r="C165" s="10" t="s">
@@ -8704,29 +8705,29 @@
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A166" s="32"/>
-      <c r="B166" s="33"/>
+      <c r="A166" s="26"/>
+      <c r="B166" s="27"/>
       <c r="C166" s="10" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A167" s="32"/>
-      <c r="B167" s="33"/>
+      <c r="A167" s="26"/>
+      <c r="B167" s="27"/>
       <c r="C167" s="10" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A168" s="32"/>
-      <c r="B168" s="33"/>
+      <c r="A168" s="26"/>
+      <c r="B168" s="27"/>
       <c r="C168" s="10" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A169" s="32"/>
-      <c r="B169" s="33"/>
+      <c r="A169" s="26"/>
+      <c r="B169" s="27"/>
       <c r="C169" s="10" t="s">
         <v>323</v>
       </c>
@@ -8743,22 +8744,22 @@
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A171" s="32" t="s">
+      <c r="A171" s="26" t="s">
         <v>327</v>
       </c>
       <c r="B171" s="10" t="s">
         <v>328</v>
       </c>
-      <c r="C171" s="33" t="s">
+      <c r="C171" s="27" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A172" s="32"/>
+      <c r="A172" s="26"/>
       <c r="B172" s="10" t="s">
         <v>329</v>
       </c>
-      <c r="C172" s="33"/>
+      <c r="C172" s="27"/>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="11" t="s">
@@ -8772,40 +8773,40 @@
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A174" s="32" t="s">
+      <c r="A174" s="26" t="s">
         <v>334</v>
       </c>
       <c r="B174" s="10" t="s">
         <v>335</v>
       </c>
-      <c r="C174" s="33" t="s">
+      <c r="C174" s="27" t="s">
         <v>337</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A175" s="32"/>
+      <c r="A175" s="26"/>
       <c r="B175" s="10" t="s">
         <v>336</v>
       </c>
-      <c r="C175" s="33"/>
+      <c r="C175" s="27"/>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A176" s="32" t="s">
+      <c r="A176" s="26" t="s">
         <v>338</v>
       </c>
       <c r="B176" s="10" t="s">
         <v>339</v>
       </c>
-      <c r="C176" s="33" t="s">
+      <c r="C176" s="27" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A177" s="32"/>
+      <c r="A177" s="26"/>
       <c r="B177" s="10" t="s">
         <v>340</v>
       </c>
-      <c r="C177" s="33"/>
+      <c r="C177" s="27"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="11" t="s">
@@ -8830,7 +8831,7 @@
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A180" s="32" t="s">
+      <c r="A180" s="26" t="s">
         <v>348</v>
       </c>
       <c r="B180" s="10" t="s">
@@ -8841,7 +8842,7 @@
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A181" s="32"/>
+      <c r="A181" s="26"/>
       <c r="B181" s="10" t="s">
         <v>350</v>
       </c>
@@ -8850,10 +8851,10 @@
       </c>
     </row>
     <row r="182" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A182" s="32" t="s">
+      <c r="A182" s="26" t="s">
         <v>353</v>
       </c>
-      <c r="B182" s="33" t="s">
+      <c r="B182" s="27" t="s">
         <v>354</v>
       </c>
       <c r="C182" s="9" t="s">
@@ -8861,17 +8862,17 @@
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A183" s="32"/>
-      <c r="B183" s="33"/>
+      <c r="A183" s="26"/>
+      <c r="B183" s="27"/>
       <c r="C183" s="10" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A184" s="32" t="s">
+      <c r="A184" s="26" t="s">
         <v>357</v>
       </c>
-      <c r="B184" s="33" t="s">
+      <c r="B184" s="27" t="s">
         <v>358</v>
       </c>
       <c r="C184" s="10" t="s">
@@ -8879,17 +8880,17 @@
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A185" s="32"/>
-      <c r="B185" s="33"/>
+      <c r="A185" s="26"/>
+      <c r="B185" s="27"/>
       <c r="C185" s="10" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A186" s="32" t="s">
+      <c r="A186" s="26" t="s">
         <v>360</v>
       </c>
-      <c r="B186" s="33" t="s">
+      <c r="B186" s="27" t="s">
         <v>361</v>
       </c>
       <c r="C186" s="10" t="s">
@@ -8897,54 +8898,54 @@
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A187" s="32"/>
-      <c r="B187" s="33"/>
+      <c r="A187" s="26"/>
+      <c r="B187" s="27"/>
       <c r="C187" s="10" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A188" s="32"/>
-      <c r="B188" s="33"/>
+      <c r="A188" s="26"/>
+      <c r="B188" s="27"/>
       <c r="C188" s="10" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A189" s="32" t="s">
+      <c r="A189" s="26" t="s">
         <v>365</v>
       </c>
       <c r="B189" s="10" t="s">
         <v>366</v>
       </c>
-      <c r="C189" s="33" t="s">
+      <c r="C189" s="27" t="s">
         <v>368</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A190" s="32"/>
+      <c r="A190" s="26"/>
       <c r="B190" s="10" t="s">
         <v>367</v>
       </c>
-      <c r="C190" s="33"/>
+      <c r="C190" s="27"/>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A191" s="32" t="s">
+      <c r="A191" s="26" t="s">
         <v>369</v>
       </c>
       <c r="B191" s="10" t="s">
         <v>370</v>
       </c>
-      <c r="C191" s="33" t="s">
+      <c r="C191" s="27" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A192" s="32"/>
+      <c r="A192" s="26"/>
       <c r="B192" s="10" t="s">
         <v>371</v>
       </c>
-      <c r="C192" s="33"/>
+      <c r="C192" s="27"/>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" s="11" t="s">
@@ -8958,22 +8959,22 @@
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A194" s="32" t="s">
+      <c r="A194" s="26" t="s">
         <v>376</v>
       </c>
       <c r="B194" s="10" t="s">
         <v>377</v>
       </c>
-      <c r="C194" s="33" t="s">
+      <c r="C194" s="27" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A195" s="32"/>
+      <c r="A195" s="26"/>
       <c r="B195" s="10" t="s">
         <v>378</v>
       </c>
-      <c r="C195" s="33"/>
+      <c r="C195" s="27"/>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" s="11" t="s">
@@ -8987,65 +8988,65 @@
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A197" s="32" t="s">
+      <c r="A197" s="26" t="s">
         <v>383</v>
       </c>
       <c r="B197" s="10" t="s">
         <v>384</v>
       </c>
-      <c r="C197" s="33" t="s">
+      <c r="C197" s="27" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A198" s="32"/>
+      <c r="A198" s="26"/>
       <c r="B198" s="10" t="s">
         <v>385</v>
       </c>
-      <c r="C198" s="33"/>
+      <c r="C198" s="27"/>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A199" s="32" t="s">
+      <c r="A199" s="26" t="s">
         <v>387</v>
       </c>
       <c r="B199" s="10" t="s">
         <v>388</v>
       </c>
-      <c r="C199" s="33" t="s">
+      <c r="C199" s="27" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A200" s="32"/>
+      <c r="A200" s="26"/>
       <c r="B200" s="12" t="s">
         <v>389</v>
       </c>
-      <c r="C200" s="33"/>
+      <c r="C200" s="27"/>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A201" s="32"/>
+      <c r="A201" s="26"/>
       <c r="B201" s="10" t="s">
         <v>390</v>
       </c>
-      <c r="C201" s="33"/>
+      <c r="C201" s="27"/>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A202" s="32" t="s">
+      <c r="A202" s="26" t="s">
         <v>392</v>
       </c>
       <c r="B202" s="10" t="s">
         <v>393</v>
       </c>
-      <c r="C202" s="33" t="s">
+      <c r="C202" s="27" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A203" s="32"/>
+      <c r="A203" s="26"/>
       <c r="B203" s="10" t="s">
         <v>394</v>
       </c>
-      <c r="C203" s="33"/>
+      <c r="C203" s="27"/>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" s="11" t="s">
@@ -9081,43 +9082,43 @@
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A207" s="32" t="s">
+      <c r="A207" s="26" t="s">
         <v>405</v>
       </c>
       <c r="B207" s="10" t="s">
         <v>406</v>
       </c>
-      <c r="C207" s="33" t="s">
+      <c r="C207" s="27" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A208" s="32"/>
+      <c r="A208" s="26"/>
       <c r="B208" s="10" t="s">
         <v>407</v>
       </c>
-      <c r="C208" s="33"/>
+      <c r="C208" s="27"/>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A209" s="32" t="s">
+      <c r="A209" s="26" t="s">
         <v>409</v>
       </c>
       <c r="B209" s="10" t="s">
         <v>410</v>
       </c>
-      <c r="C209" s="33" t="s">
+      <c r="C209" s="27" t="s">
         <v>412</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A210" s="32"/>
+      <c r="A210" s="26"/>
       <c r="B210" s="10" t="s">
         <v>411</v>
       </c>
-      <c r="C210" s="33"/>
+      <c r="C210" s="27"/>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A211" s="32" t="s">
+      <c r="A211" s="26" t="s">
         <v>413</v>
       </c>
       <c r="B211" s="10" t="s">
@@ -9128,7 +9129,7 @@
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A212" s="32"/>
+      <c r="A212" s="26"/>
       <c r="B212" s="10" t="s">
         <v>415</v>
       </c>
@@ -9137,76 +9138,76 @@
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A213" s="32" t="s">
+      <c r="A213" s="26" t="s">
         <v>418</v>
       </c>
       <c r="B213" s="10" t="s">
         <v>419</v>
       </c>
-      <c r="C213" s="33" t="s">
+      <c r="C213" s="27" t="s">
         <v>421</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A214" s="32"/>
+      <c r="A214" s="26"/>
       <c r="B214" s="10" t="s">
         <v>420</v>
       </c>
-      <c r="C214" s="33"/>
+      <c r="C214" s="27"/>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A215" s="32" t="s">
+      <c r="A215" s="26" t="s">
         <v>422</v>
       </c>
       <c r="B215" s="10" t="s">
         <v>423</v>
       </c>
-      <c r="C215" s="33" t="s">
+      <c r="C215" s="27" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A216" s="32"/>
+      <c r="A216" s="26"/>
       <c r="B216" s="10" t="s">
         <v>424</v>
       </c>
-      <c r="C216" s="33"/>
+      <c r="C216" s="27"/>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A217" s="32" t="s">
+      <c r="A217" s="26" t="s">
         <v>426</v>
       </c>
       <c r="B217" s="10" t="s">
         <v>427</v>
       </c>
-      <c r="C217" s="33" t="s">
+      <c r="C217" s="27" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A218" s="32"/>
+      <c r="A218" s="26"/>
       <c r="B218" s="10" t="s">
         <v>428</v>
       </c>
-      <c r="C218" s="33"/>
+      <c r="C218" s="27"/>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A219" s="32" t="s">
+      <c r="A219" s="26" t="s">
         <v>430</v>
       </c>
       <c r="B219" s="10" t="s">
         <v>431</v>
       </c>
-      <c r="C219" s="33" t="s">
+      <c r="C219" s="27" t="s">
         <v>433</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A220" s="32"/>
+      <c r="A220" s="26"/>
       <c r="B220" s="10" t="s">
         <v>432</v>
       </c>
-      <c r="C220" s="33"/>
+      <c r="C220" s="27"/>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A221" s="11" t="s">
@@ -9220,10 +9221,10 @@
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A222" s="32" t="s">
+      <c r="A222" s="26" t="s">
         <v>437</v>
       </c>
-      <c r="B222" s="33" t="s">
+      <c r="B222" s="27" t="s">
         <v>438</v>
       </c>
       <c r="C222" s="10" t="s">
@@ -9231,17 +9232,17 @@
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A223" s="32"/>
-      <c r="B223" s="33"/>
+      <c r="A223" s="26"/>
+      <c r="B223" s="27"/>
       <c r="C223" s="10" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A224" s="32" t="s">
+      <c r="A224" s="26" t="s">
         <v>441</v>
       </c>
-      <c r="B224" s="33" t="s">
+      <c r="B224" s="27" t="s">
         <v>442</v>
       </c>
       <c r="C224" s="10" t="s">
@@ -9249,24 +9250,24 @@
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A225" s="32"/>
-      <c r="B225" s="33"/>
+      <c r="A225" s="26"/>
+      <c r="B225" s="27"/>
       <c r="C225" s="10" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A226" s="32"/>
-      <c r="B226" s="33"/>
+      <c r="A226" s="26"/>
+      <c r="B226" s="27"/>
       <c r="C226" s="10" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A227" s="32" t="s">
+      <c r="A227" s="26" t="s">
         <v>446</v>
       </c>
-      <c r="B227" s="33" t="s">
+      <c r="B227" s="27" t="s">
         <v>447</v>
       </c>
       <c r="C227" s="10" t="s">
@@ -9274,21 +9275,21 @@
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A228" s="32"/>
-      <c r="B228" s="33"/>
+      <c r="A228" s="26"/>
+      <c r="B228" s="27"/>
       <c r="C228" s="10" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A229" s="32"/>
-      <c r="B229" s="33"/>
+      <c r="A229" s="26"/>
+      <c r="B229" s="27"/>
       <c r="C229" s="10" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A230" s="32" t="s">
+      <c r="A230" s="26" t="s">
         <v>449</v>
       </c>
       <c r="B230" s="10" t="s">
@@ -9299,7 +9300,7 @@
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A231" s="32"/>
+      <c r="A231" s="26"/>
       <c r="B231" s="10" t="s">
         <v>451</v>
       </c>
@@ -9308,61 +9309,61 @@
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A232" s="32"/>
+      <c r="A232" s="26"/>
       <c r="C232" s="10" t="s">
         <v>454</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A233" s="32"/>
+      <c r="A233" s="26"/>
       <c r="C233" s="10" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A234" s="32"/>
+      <c r="A234" s="26"/>
       <c r="C234" s="10" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A235" s="32" t="s">
+      <c r="A235" s="26" t="s">
         <v>455</v>
       </c>
       <c r="B235" s="10" t="s">
         <v>456</v>
       </c>
-      <c r="C235" s="33" t="s">
+      <c r="C235" s="27" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A236" s="32"/>
+      <c r="A236" s="26"/>
       <c r="B236" s="10" t="s">
         <v>457</v>
       </c>
-      <c r="C236" s="33"/>
+      <c r="C236" s="27"/>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A237" s="32" t="s">
+      <c r="A237" s="26" t="s">
         <v>459</v>
       </c>
       <c r="B237" s="10" t="s">
         <v>460</v>
       </c>
-      <c r="C237" s="33" t="s">
+      <c r="C237" s="27" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A238" s="32"/>
+      <c r="A238" s="26"/>
       <c r="B238" s="10" t="s">
         <v>461</v>
       </c>
-      <c r="C238" s="33"/>
+      <c r="C238" s="27"/>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A239" s="32" t="s">
+      <c r="A239" s="26" t="s">
         <v>463</v>
       </c>
       <c r="B239" s="10" t="s">
@@ -9373,7 +9374,7 @@
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A240" s="32"/>
+      <c r="A240" s="26"/>
       <c r="B240" s="10" t="s">
         <v>465</v>
       </c>
@@ -9382,13 +9383,13 @@
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A241" s="32"/>
+      <c r="A241" s="26"/>
       <c r="C241" s="10" t="s">
         <v>468</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A242" s="32" t="s">
+      <c r="A242" s="26" t="s">
         <v>469</v>
       </c>
       <c r="B242" s="10" t="s">
@@ -9399,7 +9400,7 @@
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A243" s="32"/>
+      <c r="A243" s="26"/>
       <c r="B243" s="10" t="s">
         <v>471</v>
       </c>
@@ -9408,7 +9409,7 @@
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A244" s="32"/>
+      <c r="A244" s="26"/>
       <c r="B244" s="10" t="s">
         <v>472</v>
       </c>
@@ -9417,7 +9418,7 @@
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A245" s="32"/>
+      <c r="A245" s="26"/>
       <c r="B245" s="10" t="s">
         <v>473</v>
       </c>
@@ -9426,60 +9427,60 @@
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A246" s="32"/>
+      <c r="A246" s="26"/>
       <c r="B246" s="10" t="s">
         <v>474</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A247" s="32"/>
+      <c r="A247" s="26"/>
       <c r="B247" s="10" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A248" s="32"/>
+      <c r="A248" s="26"/>
       <c r="B248" s="10" t="s">
         <v>476</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A249" s="32"/>
+      <c r="A249" s="26"/>
       <c r="B249" s="10" t="s">
         <v>477</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A250" s="32" t="s">
+      <c r="A250" s="26" t="s">
         <v>482</v>
       </c>
       <c r="B250" s="10" t="s">
         <v>483</v>
       </c>
-      <c r="C250" s="33" t="s">
+      <c r="C250" s="27" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A251" s="32"/>
+      <c r="A251" s="26"/>
       <c r="B251" s="10" t="s">
         <v>484</v>
       </c>
-      <c r="C251" s="33"/>
+      <c r="C251" s="27"/>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A252" s="32"/>
+      <c r="A252" s="26"/>
       <c r="B252" s="10" t="s">
         <v>485</v>
       </c>
-      <c r="C252" s="33"/>
+      <c r="C252" s="27"/>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A253" s="32"/>
+      <c r="A253" s="26"/>
       <c r="B253" s="10" t="s">
         <v>486</v>
       </c>
-      <c r="C253" s="33"/>
+      <c r="C253" s="27"/>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" s="11" t="s">
@@ -9504,25 +9505,25 @@
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A256" s="32" t="s">
+      <c r="A256" s="26" t="s">
         <v>494</v>
       </c>
       <c r="B256" s="10" t="s">
         <v>495</v>
       </c>
-      <c r="C256" s="33" t="s">
+      <c r="C256" s="27" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A257" s="32"/>
+      <c r="A257" s="26"/>
       <c r="B257" s="10" t="s">
         <v>496</v>
       </c>
-      <c r="C257" s="33"/>
+      <c r="C257" s="27"/>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A258" s="32" t="s">
+      <c r="A258" s="26" t="s">
         <v>498</v>
       </c>
       <c r="B258" s="10" t="s">
@@ -9533,7 +9534,7 @@
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A259" s="32"/>
+      <c r="A259" s="26"/>
       <c r="B259" s="10" t="s">
         <v>284</v>
       </c>
@@ -9542,16 +9543,16 @@
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A260" s="32"/>
+      <c r="A260" s="26"/>
       <c r="C260" s="10" t="s">
         <v>500</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A261" s="32" t="s">
+      <c r="A261" s="26" t="s">
         <v>501</v>
       </c>
-      <c r="B261" s="33" t="s">
+      <c r="B261" s="27" t="s">
         <v>502</v>
       </c>
       <c r="C261" s="10" t="s">
@@ -9559,24 +9560,24 @@
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A262" s="32"/>
-      <c r="B262" s="33"/>
+      <c r="A262" s="26"/>
+      <c r="B262" s="27"/>
       <c r="C262" s="10" t="s">
         <v>504</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A263" s="32"/>
-      <c r="B263" s="33"/>
+      <c r="A263" s="26"/>
+      <c r="B263" s="27"/>
       <c r="C263" s="10" t="s">
         <v>505</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A264" s="32" t="s">
+      <c r="A264" s="26" t="s">
         <v>506</v>
       </c>
-      <c r="B264" s="33" t="s">
+      <c r="B264" s="27" t="s">
         <v>507</v>
       </c>
       <c r="C264" s="10" t="s">
@@ -9584,57 +9585,57 @@
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A265" s="32"/>
-      <c r="B265" s="33"/>
+      <c r="A265" s="26"/>
+      <c r="B265" s="27"/>
       <c r="C265" s="10" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A266" s="32"/>
-      <c r="B266" s="33"/>
+      <c r="A266" s="26"/>
+      <c r="B266" s="27"/>
       <c r="C266" s="10" t="s">
         <v>510</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A267" s="32" t="s">
+      <c r="A267" s="26" t="s">
         <v>511</v>
       </c>
       <c r="B267" s="10" t="s">
         <v>512</v>
       </c>
-      <c r="C267" s="33" t="s">
+      <c r="C267" s="27" t="s">
         <v>514</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A268" s="32"/>
+      <c r="A268" s="26"/>
       <c r="B268" s="10" t="s">
         <v>513</v>
       </c>
-      <c r="C268" s="33"/>
+      <c r="C268" s="27"/>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A269" s="32" t="s">
+      <c r="A269" s="26" t="s">
         <v>515</v>
       </c>
       <c r="B269" s="10" t="s">
         <v>516</v>
       </c>
-      <c r="C269" s="33" t="s">
+      <c r="C269" s="27" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A270" s="32"/>
+      <c r="A270" s="26"/>
       <c r="B270" s="10" t="s">
         <v>517</v>
       </c>
-      <c r="C270" s="33"/>
+      <c r="C270" s="27"/>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A271" s="32" t="s">
+      <c r="A271" s="26" t="s">
         <v>519</v>
       </c>
       <c r="B271" s="10" t="s">
@@ -9645,7 +9646,7 @@
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A272" s="32"/>
+      <c r="A272" s="26"/>
       <c r="B272" s="10" t="s">
         <v>521</v>
       </c>
@@ -9654,70 +9655,70 @@
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A273" s="32"/>
+      <c r="A273" s="26"/>
       <c r="C273" s="10" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A274" s="32"/>
+      <c r="A274" s="26"/>
       <c r="C274" s="10" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A275" s="32" t="s">
+      <c r="A275" s="26" t="s">
         <v>526</v>
       </c>
       <c r="B275" s="10" t="s">
         <v>527</v>
       </c>
-      <c r="C275" s="33" t="s">
+      <c r="C275" s="27" t="s">
         <v>528</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A276" s="32"/>
+      <c r="A276" s="26"/>
       <c r="B276" s="10" t="s">
         <v>367</v>
       </c>
-      <c r="C276" s="33"/>
+      <c r="C276" s="27"/>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A277" s="32" t="s">
+      <c r="A277" s="26" t="s">
         <v>529</v>
       </c>
       <c r="B277" s="10" t="s">
         <v>530</v>
       </c>
-      <c r="C277" s="33" t="s">
+      <c r="C277" s="27" t="s">
         <v>531</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A278" s="32"/>
+      <c r="A278" s="26"/>
       <c r="B278" s="10" t="s">
         <v>367</v>
       </c>
-      <c r="C278" s="33"/>
+      <c r="C278" s="27"/>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A279" s="32" t="s">
+      <c r="A279" s="26" t="s">
         <v>532</v>
       </c>
       <c r="B279" s="10" t="s">
         <v>533</v>
       </c>
-      <c r="C279" s="33" t="s">
+      <c r="C279" s="27" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A280" s="32"/>
+      <c r="A280" s="26"/>
       <c r="B280" s="10" t="s">
         <v>534</v>
       </c>
-      <c r="C280" s="33"/>
+      <c r="C280" s="27"/>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281" s="11" t="s">
@@ -9753,22 +9754,22 @@
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A284" s="32" t="s">
+      <c r="A284" s="26" t="s">
         <v>545</v>
       </c>
       <c r="B284" s="10" t="s">
         <v>546</v>
       </c>
-      <c r="C284" s="33" t="s">
+      <c r="C284" s="27" t="s">
         <v>547</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A285" s="32"/>
+      <c r="A285" s="26"/>
       <c r="B285" s="10" t="s">
         <v>424</v>
       </c>
-      <c r="C285" s="33"/>
+      <c r="C285" s="27"/>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286" s="11" t="s">
@@ -9782,7 +9783,7 @@
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A287" s="32" t="s">
+      <c r="A287" s="26" t="s">
         <v>157</v>
       </c>
       <c r="B287" s="10" t="s">
@@ -9790,13 +9791,13 @@
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A288" s="32"/>
+      <c r="A288" s="26"/>
       <c r="B288" s="10" t="s">
         <v>552</v>
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A289" s="32" t="s">
+      <c r="A289" s="26" t="s">
         <v>157</v>
       </c>
       <c r="B289" s="10" t="s">
@@ -9804,7 +9805,7 @@
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A290" s="32"/>
+      <c r="A290" s="26"/>
       <c r="B290" s="10" t="s">
         <v>554</v>
       </c>
@@ -9946,7 +9947,7 @@
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A308" s="32" t="s">
+      <c r="A308" s="26" t="s">
         <v>157</v>
       </c>
       <c r="B308" s="10" t="s">
@@ -9954,25 +9955,25 @@
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A309" s="32"/>
+      <c r="A309" s="26"/>
       <c r="B309" s="10" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A310" s="32"/>
+      <c r="A310" s="26"/>
       <c r="B310" s="10" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A311" s="32"/>
+      <c r="A311" s="26"/>
       <c r="B311" s="10" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A312" s="32"/>
+      <c r="A312" s="26"/>
       <c r="B312" s="10" t="s">
         <v>589</v>
       </c>
@@ -10273,87 +10274,15 @@
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="A50:A56"/>
-    <mergeCell ref="C123:C124"/>
-    <mergeCell ref="A125:A126"/>
-    <mergeCell ref="C125:C126"/>
-    <mergeCell ref="A127:A128"/>
-    <mergeCell ref="C127:C128"/>
-    <mergeCell ref="A129:A136"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="A97:A100"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="A115:A118"/>
-    <mergeCell ref="A123:A124"/>
-    <mergeCell ref="A148:A160"/>
-    <mergeCell ref="A161:A164"/>
-    <mergeCell ref="A165:A169"/>
-    <mergeCell ref="B165:B169"/>
-    <mergeCell ref="A171:A172"/>
-    <mergeCell ref="C171:C172"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="A141:A142"/>
-    <mergeCell ref="A143:A145"/>
-    <mergeCell ref="A146:A147"/>
-    <mergeCell ref="C146:C147"/>
-    <mergeCell ref="A184:A185"/>
-    <mergeCell ref="B184:B185"/>
-    <mergeCell ref="A186:A188"/>
-    <mergeCell ref="B186:B188"/>
-    <mergeCell ref="A189:A190"/>
-    <mergeCell ref="C189:C190"/>
-    <mergeCell ref="A174:A175"/>
-    <mergeCell ref="C174:C175"/>
-    <mergeCell ref="A176:A177"/>
-    <mergeCell ref="C176:C177"/>
-    <mergeCell ref="A180:A181"/>
-    <mergeCell ref="A182:A183"/>
-    <mergeCell ref="B182:B183"/>
-    <mergeCell ref="A199:A201"/>
-    <mergeCell ref="C199:C201"/>
-    <mergeCell ref="A202:A203"/>
-    <mergeCell ref="C202:C203"/>
-    <mergeCell ref="A207:A208"/>
-    <mergeCell ref="C207:C208"/>
-    <mergeCell ref="A191:A192"/>
-    <mergeCell ref="C191:C192"/>
-    <mergeCell ref="A194:A195"/>
-    <mergeCell ref="C194:C195"/>
-    <mergeCell ref="A197:A198"/>
-    <mergeCell ref="C197:C198"/>
-    <mergeCell ref="A217:A218"/>
-    <mergeCell ref="C217:C218"/>
-    <mergeCell ref="A219:A220"/>
-    <mergeCell ref="C219:C220"/>
-    <mergeCell ref="A222:A223"/>
-    <mergeCell ref="B222:B223"/>
-    <mergeCell ref="A209:A210"/>
-    <mergeCell ref="C209:C210"/>
-    <mergeCell ref="A211:A212"/>
-    <mergeCell ref="A213:A214"/>
-    <mergeCell ref="C213:C214"/>
-    <mergeCell ref="A215:A216"/>
-    <mergeCell ref="C215:C216"/>
-    <mergeCell ref="C235:C236"/>
-    <mergeCell ref="A237:A238"/>
-    <mergeCell ref="C237:C238"/>
-    <mergeCell ref="A239:A241"/>
-    <mergeCell ref="A242:A249"/>
-    <mergeCell ref="A250:A253"/>
-    <mergeCell ref="C250:C253"/>
-    <mergeCell ref="A224:A226"/>
-    <mergeCell ref="B224:B226"/>
-    <mergeCell ref="A227:A229"/>
-    <mergeCell ref="B227:B229"/>
-    <mergeCell ref="A230:A234"/>
-    <mergeCell ref="A235:A236"/>
+    <mergeCell ref="A287:A288"/>
+    <mergeCell ref="A289:A290"/>
+    <mergeCell ref="A308:A312"/>
+    <mergeCell ref="A277:A278"/>
+    <mergeCell ref="C277:C278"/>
+    <mergeCell ref="A279:A280"/>
+    <mergeCell ref="C279:C280"/>
+    <mergeCell ref="A284:A285"/>
+    <mergeCell ref="C284:C285"/>
     <mergeCell ref="A267:A268"/>
     <mergeCell ref="C267:C268"/>
     <mergeCell ref="A269:A270"/>
@@ -10368,15 +10297,87 @@
     <mergeCell ref="B261:B263"/>
     <mergeCell ref="A264:A266"/>
     <mergeCell ref="B264:B266"/>
-    <mergeCell ref="A287:A288"/>
-    <mergeCell ref="A289:A290"/>
-    <mergeCell ref="A308:A312"/>
-    <mergeCell ref="A277:A278"/>
-    <mergeCell ref="C277:C278"/>
-    <mergeCell ref="A279:A280"/>
-    <mergeCell ref="C279:C280"/>
-    <mergeCell ref="A284:A285"/>
-    <mergeCell ref="C284:C285"/>
+    <mergeCell ref="C235:C236"/>
+    <mergeCell ref="A237:A238"/>
+    <mergeCell ref="C237:C238"/>
+    <mergeCell ref="A239:A241"/>
+    <mergeCell ref="A242:A249"/>
+    <mergeCell ref="A250:A253"/>
+    <mergeCell ref="C250:C253"/>
+    <mergeCell ref="A224:A226"/>
+    <mergeCell ref="B224:B226"/>
+    <mergeCell ref="A227:A229"/>
+    <mergeCell ref="B227:B229"/>
+    <mergeCell ref="A230:A234"/>
+    <mergeCell ref="A235:A236"/>
+    <mergeCell ref="A217:A218"/>
+    <mergeCell ref="C217:C218"/>
+    <mergeCell ref="A219:A220"/>
+    <mergeCell ref="C219:C220"/>
+    <mergeCell ref="A222:A223"/>
+    <mergeCell ref="B222:B223"/>
+    <mergeCell ref="A209:A210"/>
+    <mergeCell ref="C209:C210"/>
+    <mergeCell ref="A211:A212"/>
+    <mergeCell ref="A213:A214"/>
+    <mergeCell ref="C213:C214"/>
+    <mergeCell ref="A215:A216"/>
+    <mergeCell ref="C215:C216"/>
+    <mergeCell ref="A199:A201"/>
+    <mergeCell ref="C199:C201"/>
+    <mergeCell ref="A202:A203"/>
+    <mergeCell ref="C202:C203"/>
+    <mergeCell ref="A207:A208"/>
+    <mergeCell ref="C207:C208"/>
+    <mergeCell ref="A191:A192"/>
+    <mergeCell ref="C191:C192"/>
+    <mergeCell ref="A194:A195"/>
+    <mergeCell ref="C194:C195"/>
+    <mergeCell ref="A197:A198"/>
+    <mergeCell ref="C197:C198"/>
+    <mergeCell ref="A184:A185"/>
+    <mergeCell ref="B184:B185"/>
+    <mergeCell ref="A186:A188"/>
+    <mergeCell ref="B186:B188"/>
+    <mergeCell ref="A189:A190"/>
+    <mergeCell ref="C189:C190"/>
+    <mergeCell ref="A174:A175"/>
+    <mergeCell ref="C174:C175"/>
+    <mergeCell ref="A176:A177"/>
+    <mergeCell ref="C176:C177"/>
+    <mergeCell ref="A180:A181"/>
+    <mergeCell ref="A182:A183"/>
+    <mergeCell ref="B182:B183"/>
+    <mergeCell ref="A148:A160"/>
+    <mergeCell ref="A161:A164"/>
+    <mergeCell ref="A165:A169"/>
+    <mergeCell ref="B165:B169"/>
+    <mergeCell ref="A171:A172"/>
+    <mergeCell ref="C171:C172"/>
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="A141:A142"/>
+    <mergeCell ref="A143:A145"/>
+    <mergeCell ref="A146:A147"/>
+    <mergeCell ref="C146:C147"/>
+    <mergeCell ref="A127:A128"/>
+    <mergeCell ref="C127:C128"/>
+    <mergeCell ref="A129:A136"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="A97:A100"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="A115:A118"/>
+    <mergeCell ref="A123:A124"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A50:A56"/>
+    <mergeCell ref="C123:C124"/>
+    <mergeCell ref="A125:A126"/>
+    <mergeCell ref="C125:C126"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Several cleanup elements, including a couple of new files.
</commit_message>
<xml_diff>
--- a/data-raw/queries_wg2_ch05.xlsx
+++ b/data-raw/queries_wg2_ch05.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/citationManagement/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31727675-D6EA-A641-B3BF-DE52586DC8BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92446A09-B61E-9E41-92A7-79F79FCC2132}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38680" yWindow="10980" windowWidth="37300" windowHeight="29060" xr2:uid="{AEACCC75-8DEC-AC42-A6C7-72B5A2F10F93}"/>
+    <workbookView xWindow="29900" yWindow="8560" windowWidth="37300" windowHeight="29060" activeTab="3" xr2:uid="{AEACCC75-8DEC-AC42-A6C7-72B5A2F10F93}"/>
   </bookViews>
   <sheets>
     <sheet name="baseQueries" sheetId="1" r:id="rId1"/>
@@ -5183,9 +5183,6 @@
     <t>Potato* OR "Solanum tuberosum" OR sweetpotato* OR "sweet potat*" OR "Ipomoea batatas" OR cassava OR "Manihot esculenta" OR turnip* OR carrot* OR beetroot OR radish* OR yam* OR Dioscorea OR taro* OR cocoyam* OR yautia OR onion* OR garlic OR ginger</t>
   </si>
   <si>
-    <t xml:space="preserve">"sugar cane" OR sugarcane OR "Saccharum officinarum" OR "sugar beet" OR Beta vulgaris </t>
-  </si>
-  <si>
     <t>"oil crop*" OR rapeseed OR "rape seed" OR canola OR "Brassica napus" OR sunflower OR "sun flower" OR "Helianthus annuus" OR sesame OR "Sesamum indicum" OR "chinese tallow" OR "Triadica sebifera" OR safflower OR linseed OR "castor oil" OR "poppy oil" OR "poppyseed oil"</t>
   </si>
   <si>
@@ -5205,9 +5202,6 @@
   </si>
   <si>
     <t>barley OR oats OR triticale OR sorghum* OR millet* OR rye* OR buckwheat* OR fonio* OR teff OR Quinoa</t>
-  </si>
-  <si>
-    <t>almond* OR cashew* OR hazel* OR walnut* OR pistachio* OR macadamia* OR chestnut* OR Areca OR "Karite nut*" OR sheanut* OR "Vitellaria paradoxa" OR kola* OR "brazil nut" OR "Bertholletia excelsa" OR "pine nut"</t>
   </si>
   <si>
     <t>pig OR hog OR swine OR poultry OR chicken OR broilers OR ruminant OR sheep OR goat OR cattle OR buffalo OR beef OR pork OR lamb OR mutton</t>
@@ -5502,9 +5496,6 @@
     <t>searchStrings.climateChangeSource</t>
   </si>
   <si>
-    <t>"heat stress" OR "yield decline" OR "yield variability" OR "nutrition* quality"</t>
-  </si>
-  <si>
     <t>searchStrings.climateImpacts</t>
   </si>
   <si>
@@ -5559,9 +5550,6 @@
     <t>maize OR corn</t>
   </si>
   <si>
-    <t>"greenhouse gas" OR "global warming" OR "climate change" OR "climate variability" OR "climate warming"</t>
-  </si>
-  <si>
     <t>geneticEngCropMain</t>
   </si>
   <si>
@@ -5628,12 +5616,6 @@
     <t>(livestock OR ruminant OR cattle OR beef OR goat OR sheep OR pig OR shoat OR swine OR pork OR chicken OR poultry) AND (pasture OR grass* OR rangeland OR feed OR forag* OR hay OR silage)</t>
   </si>
   <si>
-    <t>c("greenhouse gas", "global warming", "climate change", "climate variability", "climate warming")</t>
-  </si>
-  <si>
-    <t>"climate hazard" OR "extreme weather" OR "heat wave" OR "precipitation variability" OR "rainfall variability" OR "temperature  variability" OR "sea level rise" OR drought OR "intense rainfall" OR flood*</t>
-  </si>
-  <si>
     <t>searchStrings.mitigation</t>
   </si>
   <si>
@@ -5914,6 +5896,24 @@
   </si>
   <si>
     <t>(crop OR plant) AND (pest* OR insect* OR fung* OR weed* OR  locust  OR  "desert locust"  OR  "Schistocerca gregaria")</t>
+  </si>
+  <si>
+    <t>"sugar cane" OR sugarcane OR "Saccharum officinarum" OR "sugar beet" OR "Beta vulgaris"</t>
+  </si>
+  <si>
+    <t>almond* OR cashew* OR hazel* OR walnut* OR pistachio* OR macadamia* OR chestnut* OR Areca OR "Karite nut*" OR sheanut* OR "Vitellaria paradoxa" OR "kola nut" OR "kola nuts" OR "kola tree" OR "kola trees" OR "brazil nut" OR "Bertholletia excelsa" OR "pine nut"</t>
+  </si>
+  <si>
+    <t>{greenhouse gas} OR {global warming} OR {climate change} OR {climatic change} OR {climate variability} OR {climate warming}</t>
+  </si>
+  <si>
+    <t>c("greenhouse gas", "global warming", "climate change", "climatic change", "climate variability", "climate warming")</t>
+  </si>
+  <si>
+    <t>{climate hazard} OR {extreme weather} OR {heat wave} OR {precipitation variability} OR {rainfall variability} OR {temperature  variability} OR {sea level rise} OR drought OR {intense rainfall} OR flood*</t>
+  </si>
+  <si>
+    <t>{heat stress} OR {yield decline} OR {yield variability} OR {nutritional quality}</t>
   </si>
 </sst>
 </file>
@@ -6619,8 +6619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11F86CE5-FC64-FA44-BB0B-0B6C961403B7}">
   <dimension ref="A1:I109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView topLeftCell="A51" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -6651,16 +6651,16 @@
         <v>7</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="G1" s="13" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="I1" s="13" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="32">
@@ -6668,25 +6668,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="26" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>873</v>
+        <v>867</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>907</v>
+        <v>901</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="I2" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="80">
@@ -6698,10 +6698,10 @@
         <v>678</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>845</v>
+        <v>841</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>915</v>
+        <v>909</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="48">
@@ -6713,10 +6713,10 @@
         <v>678</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>846</v>
+        <v>842</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>888</v>
+        <v>882</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="64">
@@ -6728,10 +6728,10 @@
         <v>678</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>876</v>
+        <v>870</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="32">
@@ -6744,22 +6744,22 @@
       </c>
       <c r="C6" s="47"/>
       <c r="D6" s="47" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="E6" s="48" t="s">
-        <v>919</v>
+        <v>913</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G6" s="13" t="s">
         <v>78</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="32">
@@ -6775,19 +6775,19 @@
         <v>78</v>
       </c>
       <c r="E7" s="48" t="s">
-        <v>909</v>
+        <v>903</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="G7" s="13" t="s">
         <v>78</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="32">
@@ -6803,19 +6803,19 @@
         <v>79</v>
       </c>
       <c r="E8" s="48" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="G8" s="13" t="s">
         <v>78</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="16">
@@ -6828,22 +6828,22 @@
       </c>
       <c r="C9" s="47"/>
       <c r="D9" s="47" t="s">
-        <v>953</v>
+        <v>947</v>
       </c>
       <c r="E9" s="48" t="s">
-        <v>954</v>
+        <v>948</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="G9" s="34" t="s">
         <v>78</v>
       </c>
       <c r="H9" s="34" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="I9" s="34" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="16">
@@ -6856,13 +6856,13 @@
       </c>
       <c r="C10" s="47"/>
       <c r="D10" s="47" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="E10" s="48" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>78</v>
@@ -6880,10 +6880,10 @@
         <v>6</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>895</v>
+        <v>889</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>78</v>
@@ -6899,13 +6899,13 @@
       </c>
       <c r="C12" s="50"/>
       <c r="D12" s="50" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="E12" s="49" t="s">
-        <v>868</v>
+        <v>862</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G12" s="19" t="s">
         <v>78</v>
@@ -6923,13 +6923,13 @@
       </c>
       <c r="C13" s="50"/>
       <c r="D13" s="50" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="E13" s="49" t="s">
-        <v>912</v>
+        <v>906</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="G13" s="19" t="s">
         <v>78</v>
@@ -6947,13 +6947,13 @@
       </c>
       <c r="C14" s="50"/>
       <c r="D14" s="50" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="E14" s="49" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G14" s="19" t="s">
         <v>78</v>
@@ -6970,10 +6970,10 @@
         <v>678</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>843</v>
+        <v>839</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>875</v>
+        <v>869</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>78</v>
@@ -6988,13 +6988,13 @@
         <v>678</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>844</v>
+        <v>840</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>877</v>
+        <v>871</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G16" s="13" t="s">
         <v>78</v>
@@ -7009,13 +7009,13 @@
         <v>678</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>889</v>
+        <v>883</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G17" s="13" t="s">
         <v>78</v>
@@ -7030,13 +7030,13 @@
         <v>678</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>878</v>
+        <v>872</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G18" s="13" t="s">
         <v>78</v>
@@ -7052,13 +7052,13 @@
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="13" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>879</v>
+        <v>873</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>78</v>
@@ -7082,7 +7082,7 @@
         <v>645</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G20" s="13" t="s">
         <v>78</v>
@@ -7103,10 +7103,10 @@
         <v>87</v>
       </c>
       <c r="E21" s="24" t="s">
-        <v>890</v>
+        <v>884</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="G21" s="19" t="s">
         <v>78</v>
@@ -7127,10 +7127,10 @@
         <v>690</v>
       </c>
       <c r="E22" s="23" t="s">
-        <v>910</v>
+        <v>904</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="G22" s="19" t="s">
         <v>78</v>
@@ -7154,7 +7154,7 @@
         <v>703</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="G23" s="19" t="s">
         <v>78</v>
@@ -7171,13 +7171,13 @@
         <v>682</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>925</v>
+        <v>919</v>
       </c>
       <c r="E24" s="47" t="s">
-        <v>928</v>
+        <v>922</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="G24" s="13" t="s">
         <v>78</v>
@@ -7192,13 +7192,13 @@
         <v>682</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>926</v>
+        <v>920</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>927</v>
+        <v>921</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="G25" s="13" t="s">
         <v>78</v>
@@ -7213,13 +7213,13 @@
         <v>682</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>929</v>
+        <v>923</v>
       </c>
       <c r="E26" s="53" t="s">
-        <v>930</v>
+        <v>924</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="G26" s="13" t="s">
         <v>78</v>
@@ -7240,16 +7240,16 @@
         <v>663</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="16">
@@ -7267,16 +7267,16 @@
         <v>662</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="16">
@@ -7294,16 +7294,16 @@
         <v>698</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="32">
@@ -7318,19 +7318,19 @@
         <v>69</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>921</v>
+        <v>915</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="32">
@@ -7345,19 +7345,19 @@
         <v>666</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>924</v>
+        <v>918</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G31" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="32">
@@ -7372,19 +7372,19 @@
         <v>665</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>900</v>
+        <v>894</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="32">
@@ -7399,19 +7399,19 @@
         <v>70</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
     </row>
     <row r="34" spans="1:9" ht="16">
@@ -7423,22 +7423,22 @@
         <v>696</v>
       </c>
       <c r="D34" s="13" t="s">
+        <v>802</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>804</v>
       </c>
-      <c r="E34" s="7" t="s">
-        <v>806</v>
-      </c>
       <c r="F34" s="13" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="G34" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="32">
@@ -7453,19 +7453,19 @@
         <v>664</v>
       </c>
       <c r="E35" s="32" t="s">
-        <v>901</v>
+        <v>895</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="I35" s="13" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
     </row>
     <row r="36" spans="1:9" ht="32">
@@ -7480,13 +7480,13 @@
         <v>77</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>880</v>
+        <v>874</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="37" spans="1:9" ht="16">
@@ -7501,16 +7501,16 @@
         <v>715</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="16">
@@ -7522,16 +7522,16 @@
         <v>678</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>920</v>
+        <v>914</v>
       </c>
       <c r="F38" s="13" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="G38" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="39" spans="1:9" ht="32">
@@ -7546,13 +7546,13 @@
         <v>694</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>881</v>
+        <v>875</v>
       </c>
       <c r="F39" s="13" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="G39" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="40" spans="1:9" ht="48">
@@ -7567,13 +7567,13 @@
         <v>73</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="F40" s="13" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="G40" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="16">
@@ -7588,13 +7588,13 @@
         <v>4</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>869</v>
+        <v>863</v>
       </c>
       <c r="F41" s="13" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="G41" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="32">
@@ -7609,16 +7609,16 @@
         <v>716</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="E42" s="14" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="F42" s="13" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="G42" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="16">
@@ -7633,13 +7633,13 @@
         <v>90</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>860</v>
+        <v>856</v>
       </c>
       <c r="F43" s="13" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="G43" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="32">
@@ -7651,16 +7651,16 @@
         <v>678</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>882</v>
+        <v>876</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="G44" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="16">
@@ -7675,13 +7675,13 @@
         <v>88</v>
       </c>
       <c r="E45" s="21" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G45" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="46" spans="1:9" ht="48">
@@ -7696,16 +7696,16 @@
         <v>712</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="F46" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G46" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="16">
@@ -7720,13 +7720,13 @@
         <v>75</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="F47" s="13" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="G47" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="48">
@@ -7741,16 +7741,16 @@
         <v>715</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="F48" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G48" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="16">
@@ -7765,16 +7765,16 @@
         <v>715</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="F49" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G49" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="16">
@@ -7787,16 +7787,16 @@
       </c>
       <c r="C50" s="19"/>
       <c r="D50" s="19" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="E50" s="23" t="s">
-        <v>870</v>
+        <v>864</v>
       </c>
       <c r="F50" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G50" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="32">
@@ -7811,13 +7811,13 @@
         <v>673</v>
       </c>
       <c r="E51" s="20" t="s">
-        <v>960</v>
+        <v>954</v>
       </c>
       <c r="F51" s="13" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G51" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="16">
@@ -7829,16 +7829,16 @@
         <v>678</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="F52" s="13" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="G52" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="16">
@@ -7856,10 +7856,10 @@
         <v>76</v>
       </c>
       <c r="F53" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G53" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="48">
@@ -7874,16 +7874,16 @@
         <v>713</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="E54" s="14" t="s">
         <v>718</v>
       </c>
       <c r="F54" s="13" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="G54" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="32">
@@ -7898,16 +7898,16 @@
         <v>711</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="E55" s="14" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="F55" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G55" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="16">
@@ -7925,13 +7925,13 @@
         <v>641</v>
       </c>
       <c r="E56" s="14" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="F56" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G56" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="48">
@@ -7943,19 +7943,19 @@
         <v>678</v>
       </c>
       <c r="C57" s="16" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="E57" s="14" t="s">
-        <v>872</v>
+        <v>866</v>
       </c>
       <c r="F57" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G57" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="16">
@@ -7970,16 +7970,16 @@
         <v>712</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="E58" s="14" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="F58" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G58" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="48">
@@ -7994,16 +7994,16 @@
         <v>715</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="E59" s="14" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="F59" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G59" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="16">
@@ -8018,16 +8018,16 @@
         <v>714</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="E60" s="14" t="s">
-        <v>719</v>
+        <v>955</v>
       </c>
       <c r="F60" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G60" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="61" spans="1:7" ht="16">
@@ -8042,16 +8042,16 @@
         <v>707</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="E61" s="22" t="s">
         <v>708</v>
       </c>
       <c r="F61" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G61" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="16">
@@ -8066,16 +8066,16 @@
         <v>707</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="E62" s="22" t="s">
         <v>709</v>
       </c>
       <c r="F62" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G62" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="63" spans="1:7" ht="96">
@@ -8090,16 +8090,16 @@
         <v>707</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="E63" s="22" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="F63" s="13" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="G63" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="32">
@@ -8114,16 +8114,16 @@
         <v>710</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="E64" s="14" t="s">
         <v>717</v>
       </c>
       <c r="F64" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G64" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="65" spans="1:9" s="18" customFormat="1" ht="48">
@@ -8138,16 +8138,16 @@
         <v>707</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="E65" s="22" t="s">
-        <v>727</v>
+        <v>956</v>
       </c>
       <c r="F65" s="13" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G65" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H65" s="13"/>
       <c r="I65" s="13"/>
@@ -8164,16 +8164,16 @@
         <v>711</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="E66" s="14" t="s">
-        <v>871</v>
+        <v>865</v>
       </c>
       <c r="F66" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="G66" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H66" s="13"/>
       <c r="I66" s="13"/>
@@ -8194,10 +8194,10 @@
         <v>74</v>
       </c>
       <c r="F67" s="13" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="G67" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H67" s="13"/>
       <c r="I67" s="13"/>
@@ -8215,13 +8215,13 @@
         <v>693</v>
       </c>
       <c r="E68" s="7" t="s">
-        <v>906</v>
+        <v>900</v>
       </c>
       <c r="F68" s="13" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="G68" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H68" s="13"/>
       <c r="I68" s="13"/>
@@ -8239,13 +8239,13 @@
         <v>687</v>
       </c>
       <c r="E69" s="7" t="s">
-        <v>891</v>
+        <v>885</v>
       </c>
       <c r="F69" s="13" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="G69" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H69" s="13"/>
       <c r="I69" s="13"/>
@@ -8266,10 +8266,10 @@
         <v>699</v>
       </c>
       <c r="F70" s="13" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="G70" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H70" s="13"/>
       <c r="I70" s="13"/>
@@ -8284,16 +8284,16 @@
       </c>
       <c r="C71" s="13"/>
       <c r="D71" s="13" t="s">
-        <v>861</v>
+        <v>857</v>
       </c>
       <c r="E71" s="21" t="s">
-        <v>908</v>
+        <v>902</v>
       </c>
       <c r="F71" s="13" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="G71" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H71" s="19"/>
       <c r="I71" s="19"/>
@@ -8311,13 +8311,13 @@
         <v>68</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>911</v>
+        <v>905</v>
       </c>
       <c r="F72" s="19" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="G72" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H72" s="19"/>
       <c r="I72" s="19"/>
@@ -8335,13 +8335,13 @@
         <v>5</v>
       </c>
       <c r="E73" s="21" t="s">
-        <v>886</v>
+        <v>880</v>
       </c>
       <c r="F73" s="19" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="G73" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H73" s="19"/>
       <c r="I73" s="19"/>
@@ -8362,10 +8362,10 @@
         <v>700</v>
       </c>
       <c r="F74" s="19" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="G74" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H74" s="19"/>
       <c r="I74" s="19"/>
@@ -8383,13 +8383,13 @@
         <v>0</v>
       </c>
       <c r="E75" s="21" t="s">
-        <v>892</v>
+        <v>886</v>
       </c>
       <c r="F75" s="19" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="G75" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H75" s="19"/>
       <c r="I75" s="19"/>
@@ -8407,13 +8407,13 @@
         <v>686</v>
       </c>
       <c r="E76" s="7" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="F76" s="19" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="G76" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H76" s="19"/>
       <c r="I76" s="19"/>
@@ -8431,13 +8431,13 @@
         <v>688</v>
       </c>
       <c r="E77" s="23" t="s">
-        <v>913</v>
+        <v>907</v>
       </c>
       <c r="F77" s="19" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="G77" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H77" s="19"/>
       <c r="I77" s="19"/>
@@ -8458,10 +8458,10 @@
         <v>697</v>
       </c>
       <c r="F78" s="19" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="G78" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H78" s="19"/>
       <c r="I78" s="19"/>
@@ -8479,13 +8479,13 @@
         <v>89</v>
       </c>
       <c r="E79" s="24" t="s">
-        <v>862</v>
+        <v>858</v>
       </c>
       <c r="F79" s="19" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="G79" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H79" s="19"/>
       <c r="I79" s="19"/>
@@ -8503,13 +8503,13 @@
         <v>93</v>
       </c>
       <c r="E80" s="24" t="s">
-        <v>863</v>
+        <v>859</v>
       </c>
       <c r="F80" s="19" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="G80" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H80" s="19"/>
       <c r="I80" s="19"/>
@@ -8530,10 +8530,10 @@
         <v>701</v>
       </c>
       <c r="F81" s="19" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="G81" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H81" s="19"/>
       <c r="I81" s="19"/>
@@ -8551,13 +8551,13 @@
         <v>92</v>
       </c>
       <c r="E82" s="24" t="s">
-        <v>864</v>
+        <v>860</v>
       </c>
       <c r="F82" s="19" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="G82" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H82" s="19"/>
       <c r="I82" s="19"/>
@@ -8575,13 +8575,13 @@
         <v>674</v>
       </c>
       <c r="E83" s="25" t="s">
-        <v>883</v>
+        <v>877</v>
       </c>
       <c r="F83" s="19" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="G83" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H83" s="19"/>
       <c r="I83" s="19"/>
@@ -8602,10 +8602,10 @@
         <v>702</v>
       </c>
       <c r="F84" s="19" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="G84" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H84" s="19"/>
       <c r="I84" s="19"/>
@@ -8620,16 +8620,16 @@
       </c>
       <c r="C85" s="19"/>
       <c r="D85" s="13" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="E85" s="24" t="s">
-        <v>902</v>
+        <v>896</v>
       </c>
       <c r="F85" s="19" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="G85" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H85" s="19"/>
       <c r="I85" s="19"/>
@@ -8644,16 +8644,16 @@
       </c>
       <c r="C86" s="19"/>
       <c r="D86" s="13" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="E86" s="20" t="s">
-        <v>884</v>
+        <v>878</v>
       </c>
       <c r="F86" s="19" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="G86" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H86" s="19"/>
       <c r="I86" s="19"/>
@@ -8671,13 +8671,13 @@
         <v>661</v>
       </c>
       <c r="E87" s="33" t="s">
-        <v>922</v>
+        <v>916</v>
       </c>
       <c r="F87" s="19" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="G87" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H87" s="19"/>
       <c r="I87" s="19"/>
@@ -8692,16 +8692,16 @@
       </c>
       <c r="C88" s="19"/>
       <c r="D88" s="19" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="E88" s="23" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="F88" s="19" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="G88" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="89" spans="1:9" ht="16">
@@ -8720,10 +8720,10 @@
         <v>704</v>
       </c>
       <c r="F89" s="13" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="G89" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="90" spans="1:9" ht="32">
@@ -8732,20 +8732,20 @@
         <v>89</v>
       </c>
       <c r="B90" s="29" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="C90" s="30"/>
       <c r="D90" s="30" t="s">
+        <v>816</v>
+      </c>
+      <c r="E90" s="29" t="s">
+        <v>817</v>
+      </c>
+      <c r="F90" s="30" t="s">
         <v>818</v>
       </c>
-      <c r="E90" s="29" t="s">
-        <v>819</v>
-      </c>
-      <c r="F90" s="30" t="s">
-        <v>820</v>
-      </c>
       <c r="G90" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H90" s="19"/>
       <c r="I90" s="19"/>
@@ -8763,13 +8763,13 @@
         <v>676</v>
       </c>
       <c r="E91" s="23" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="F91" s="13" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="G91" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="92" spans="1:9" ht="16">
@@ -8788,10 +8788,10 @@
         <v>705</v>
       </c>
       <c r="F92" s="19" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="G92" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="48">
@@ -8807,13 +8807,13 @@
         <v>86</v>
       </c>
       <c r="E93" s="24" t="s">
-        <v>903</v>
+        <v>897</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="G93" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="16">
@@ -8825,16 +8825,16 @@
         <v>683</v>
       </c>
       <c r="D94" s="13" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="E94" s="20" t="s">
-        <v>885</v>
+        <v>879</v>
       </c>
       <c r="F94" s="28" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="G94" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="95" spans="1:9">
@@ -8846,16 +8846,16 @@
         <v>682</v>
       </c>
       <c r="D95" s="13" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="E95" s="34" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="F95" s="28" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G95" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="96" spans="1:9" ht="16">
@@ -8871,13 +8871,13 @@
         <v>669</v>
       </c>
       <c r="E96" s="23" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="F96" s="28" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G96" s="19" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="16">
@@ -8889,16 +8889,16 @@
         <v>678</v>
       </c>
       <c r="D97" s="13" t="s">
-        <v>893</v>
+        <v>887</v>
       </c>
       <c r="E97" s="7" t="s">
-        <v>894</v>
+        <v>888</v>
       </c>
       <c r="F97" s="13" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="G97" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="48">
@@ -8910,16 +8910,16 @@
         <v>85</v>
       </c>
       <c r="D98" s="13" t="s">
-        <v>897</v>
+        <v>891</v>
       </c>
       <c r="E98" s="7" t="s">
-        <v>916</v>
+        <v>910</v>
       </c>
       <c r="F98" s="13" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="G98" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="99" spans="1:9" ht="32">
@@ -8931,22 +8931,22 @@
         <v>691</v>
       </c>
       <c r="D99" s="13" t="s">
-        <v>914</v>
+        <v>908</v>
       </c>
       <c r="E99" s="52" t="s">
-        <v>923</v>
+        <v>917</v>
       </c>
       <c r="F99" s="13" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="G99" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="H99" s="13" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="I99" s="13" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="48">
@@ -8958,16 +8958,16 @@
         <v>683</v>
       </c>
       <c r="D100" s="13" t="s">
-        <v>931</v>
+        <v>925</v>
       </c>
       <c r="E100" s="7" t="s">
-        <v>932</v>
+        <v>926</v>
       </c>
       <c r="F100" s="13" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="G100" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="101" spans="1:9" ht="16">
@@ -8979,16 +8979,16 @@
         <v>683</v>
       </c>
       <c r="D101" s="13" t="s">
-        <v>933</v>
+        <v>927</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>934</v>
+        <v>928</v>
       </c>
       <c r="F101" s="13" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="G101" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="102" spans="1:9" ht="16">
@@ -8997,19 +8997,19 @@
         <v>101</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>936</v>
+        <v>930</v>
       </c>
       <c r="D102" s="13" t="s">
-        <v>935</v>
+        <v>929</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>937</v>
+        <v>931</v>
       </c>
       <c r="F102" s="13" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="G102" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="103" spans="1:9" ht="16">
@@ -9018,19 +9018,19 @@
         <v>102</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>938</v>
+        <v>932</v>
       </c>
       <c r="D103" s="13" t="s">
-        <v>939</v>
+        <v>933</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>940</v>
+        <v>934</v>
       </c>
       <c r="F103" s="13" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="G103" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="16">
@@ -9039,16 +9039,16 @@
         <v>103</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>941</v>
+        <v>935</v>
       </c>
       <c r="D104" s="13" t="s">
-        <v>942</v>
+        <v>936</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>943</v>
+        <v>937</v>
       </c>
       <c r="F104" s="13" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
     </row>
     <row r="105" spans="1:9" ht="32">
@@ -9057,16 +9057,16 @@
         <v>104</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>944</v>
+        <v>938</v>
       </c>
       <c r="D105" s="13" t="s">
-        <v>945</v>
+        <v>939</v>
       </c>
       <c r="E105" s="54" t="s">
-        <v>946</v>
+        <v>940</v>
       </c>
       <c r="F105" s="13" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
     </row>
     <row r="106" spans="1:9" ht="16">
@@ -9075,19 +9075,19 @@
         <v>105</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>947</v>
+        <v>941</v>
       </c>
       <c r="D106" s="13" t="s">
-        <v>948</v>
+        <v>942</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>949</v>
+        <v>943</v>
       </c>
       <c r="F106" s="13" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="G106" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="16">
@@ -9096,16 +9096,16 @@
         <v>106</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>950</v>
+        <v>944</v>
       </c>
       <c r="D107" s="13" t="s">
-        <v>951</v>
+        <v>945</v>
       </c>
       <c r="E107" s="7" t="s">
-        <v>952</v>
+        <v>946</v>
       </c>
       <c r="F107" s="13" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="64">
@@ -9114,19 +9114,19 @@
         <v>107</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>957</v>
+        <v>951</v>
       </c>
       <c r="D108" s="13" t="s">
-        <v>958</v>
+        <v>952</v>
       </c>
       <c r="E108" s="7" t="s">
-        <v>959</v>
+        <v>953</v>
       </c>
       <c r="F108" s="13" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="G108" s="13" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
     </row>
     <row r="109" spans="1:9">
@@ -9160,7 +9160,7 @@
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
     </row>
   </sheetData>
@@ -9173,7 +9173,7 @@
   <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9195,7 +9195,7 @@
         <v>98</v>
       </c>
       <c r="B2" s="35" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -9203,7 +9203,7 @@
         <v>96</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -9216,42 +9216,42 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="35" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="B5" s="36" t="s">
-        <v>865</v>
+        <v>958</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="35" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>898</v>
+        <v>892</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="35" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>956</v>
+        <v>950</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="37" t="s">
-        <v>858</v>
+        <v>854</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="37" t="s">
-        <v>859</v>
+        <v>855</v>
       </c>
       <c r="B9" s="35" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -9307,7 +9307,7 @@
         <v>105</v>
       </c>
       <c r="B16" s="35" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -9315,15 +9315,15 @@
         <v>106</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>899</v>
+        <v>893</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="35" t="s">
-        <v>904</v>
+        <v>898</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>905</v>
+        <v>899</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -9331,7 +9331,7 @@
         <v>107</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -9347,7 +9347,7 @@
         <v>110</v>
       </c>
       <c r="B21" s="35" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -9379,7 +9379,7 @@
         <v>652</v>
       </c>
       <c r="B25" s="39" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -9395,7 +9395,7 @@
         <v>655</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -9435,87 +9435,87 @@
         <v>677</v>
       </c>
       <c r="B32" s="42" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
     </row>
     <row r="33" spans="1:2" s="27" customFormat="1">
       <c r="A33" s="44" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="B33" s="45" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="27" customFormat="1">
       <c r="A34" s="44" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="B34" s="45" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
     </row>
     <row r="35" spans="1:2" s="27" customFormat="1">
       <c r="A35" s="44" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="B35" s="45" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
     </row>
     <row r="36" spans="1:2" s="27" customFormat="1">
       <c r="A36" s="44" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B36" s="45" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
     </row>
     <row r="37" spans="1:2" s="27" customFormat="1">
       <c r="A37" s="44" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="B37" s="45" t="s">
-        <v>874</v>
+        <v>868</v>
       </c>
     </row>
     <row r="38" spans="1:2" s="27" customFormat="1">
       <c r="A38" s="44" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="B38" s="45" t="s">
-        <v>955</v>
+        <v>949</v>
       </c>
     </row>
     <row r="39" spans="1:2" s="27" customFormat="1">
       <c r="A39" s="44" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="B39" s="45" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" s="44" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="B40" s="45" t="s">
-        <v>896</v>
+        <v>890</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" s="44" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="B41" s="36" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="51" t="s">
-        <v>917</v>
+        <v>911</v>
       </c>
       <c r="B42" s="45" t="s">
-        <v>918</v>
+        <v>912</v>
       </c>
     </row>
   </sheetData>
@@ -9527,8 +9527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5825E51-79F8-3943-A43A-0FB9AED7F8CD}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9546,40 +9546,40 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="B2" s="31" t="s">
-        <v>842</v>
+        <v>957</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>866</v>
+        <v>959</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>867</v>
+        <v>861</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>887</v>
+        <v>881</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="B5" s="31"/>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>823</v>
+        <v>960</v>
       </c>
     </row>
   </sheetData>
@@ -9591,13 +9591,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DB3225A-4DA2-B449-9413-FA03533C994C}">
   <dimension ref="A1:C350"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:A25"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="1" max="1" width="45.33203125" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12258,15 +12258,87 @@
     </row>
   </sheetData>
   <mergeCells count="104">
-    <mergeCell ref="A287:A288"/>
-    <mergeCell ref="A289:A290"/>
-    <mergeCell ref="A308:A312"/>
-    <mergeCell ref="A277:A278"/>
-    <mergeCell ref="C277:C278"/>
-    <mergeCell ref="A279:A280"/>
-    <mergeCell ref="C279:C280"/>
-    <mergeCell ref="A284:A285"/>
-    <mergeCell ref="C284:C285"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A31:A32"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="A50:A56"/>
+    <mergeCell ref="C123:C124"/>
+    <mergeCell ref="A125:A126"/>
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="A127:A128"/>
+    <mergeCell ref="C127:C128"/>
+    <mergeCell ref="A129:A136"/>
+    <mergeCell ref="A59:A61"/>
+    <mergeCell ref="A70:A73"/>
+    <mergeCell ref="A97:A100"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="A115:A118"/>
+    <mergeCell ref="A123:A124"/>
+    <mergeCell ref="A148:A160"/>
+    <mergeCell ref="A161:A164"/>
+    <mergeCell ref="A165:A169"/>
+    <mergeCell ref="B165:B169"/>
+    <mergeCell ref="A171:A172"/>
+    <mergeCell ref="C171:C172"/>
+    <mergeCell ref="A137:A138"/>
+    <mergeCell ref="A139:A140"/>
+    <mergeCell ref="A141:A142"/>
+    <mergeCell ref="A143:A145"/>
+    <mergeCell ref="A146:A147"/>
+    <mergeCell ref="C146:C147"/>
+    <mergeCell ref="A184:A185"/>
+    <mergeCell ref="B184:B185"/>
+    <mergeCell ref="A186:A188"/>
+    <mergeCell ref="B186:B188"/>
+    <mergeCell ref="A189:A190"/>
+    <mergeCell ref="C189:C190"/>
+    <mergeCell ref="A174:A175"/>
+    <mergeCell ref="C174:C175"/>
+    <mergeCell ref="A176:A177"/>
+    <mergeCell ref="C176:C177"/>
+    <mergeCell ref="A180:A181"/>
+    <mergeCell ref="A182:A183"/>
+    <mergeCell ref="B182:B183"/>
+    <mergeCell ref="A199:A201"/>
+    <mergeCell ref="C199:C201"/>
+    <mergeCell ref="A202:A203"/>
+    <mergeCell ref="C202:C203"/>
+    <mergeCell ref="A207:A208"/>
+    <mergeCell ref="C207:C208"/>
+    <mergeCell ref="A191:A192"/>
+    <mergeCell ref="C191:C192"/>
+    <mergeCell ref="A194:A195"/>
+    <mergeCell ref="C194:C195"/>
+    <mergeCell ref="A197:A198"/>
+    <mergeCell ref="C197:C198"/>
+    <mergeCell ref="A217:A218"/>
+    <mergeCell ref="C217:C218"/>
+    <mergeCell ref="A219:A220"/>
+    <mergeCell ref="C219:C220"/>
+    <mergeCell ref="A222:A223"/>
+    <mergeCell ref="B222:B223"/>
+    <mergeCell ref="A209:A210"/>
+    <mergeCell ref="C209:C210"/>
+    <mergeCell ref="A211:A212"/>
+    <mergeCell ref="A213:A214"/>
+    <mergeCell ref="C213:C214"/>
+    <mergeCell ref="A215:A216"/>
+    <mergeCell ref="C215:C216"/>
+    <mergeCell ref="C235:C236"/>
+    <mergeCell ref="A237:A238"/>
+    <mergeCell ref="C237:C238"/>
+    <mergeCell ref="A239:A241"/>
+    <mergeCell ref="A242:A249"/>
+    <mergeCell ref="A250:A253"/>
+    <mergeCell ref="C250:C253"/>
+    <mergeCell ref="A224:A226"/>
+    <mergeCell ref="B224:B226"/>
+    <mergeCell ref="A227:A229"/>
+    <mergeCell ref="B227:B229"/>
+    <mergeCell ref="A230:A234"/>
+    <mergeCell ref="A235:A236"/>
     <mergeCell ref="A267:A268"/>
     <mergeCell ref="C267:C268"/>
     <mergeCell ref="A269:A270"/>
@@ -12281,87 +12353,15 @@
     <mergeCell ref="B261:B263"/>
     <mergeCell ref="A264:A266"/>
     <mergeCell ref="B264:B266"/>
-    <mergeCell ref="C235:C236"/>
-    <mergeCell ref="A237:A238"/>
-    <mergeCell ref="C237:C238"/>
-    <mergeCell ref="A239:A241"/>
-    <mergeCell ref="A242:A249"/>
-    <mergeCell ref="A250:A253"/>
-    <mergeCell ref="C250:C253"/>
-    <mergeCell ref="A224:A226"/>
-    <mergeCell ref="B224:B226"/>
-    <mergeCell ref="A227:A229"/>
-    <mergeCell ref="B227:B229"/>
-    <mergeCell ref="A230:A234"/>
-    <mergeCell ref="A235:A236"/>
-    <mergeCell ref="A217:A218"/>
-    <mergeCell ref="C217:C218"/>
-    <mergeCell ref="A219:A220"/>
-    <mergeCell ref="C219:C220"/>
-    <mergeCell ref="A222:A223"/>
-    <mergeCell ref="B222:B223"/>
-    <mergeCell ref="A209:A210"/>
-    <mergeCell ref="C209:C210"/>
-    <mergeCell ref="A211:A212"/>
-    <mergeCell ref="A213:A214"/>
-    <mergeCell ref="C213:C214"/>
-    <mergeCell ref="A215:A216"/>
-    <mergeCell ref="C215:C216"/>
-    <mergeCell ref="A199:A201"/>
-    <mergeCell ref="C199:C201"/>
-    <mergeCell ref="A202:A203"/>
-    <mergeCell ref="C202:C203"/>
-    <mergeCell ref="A207:A208"/>
-    <mergeCell ref="C207:C208"/>
-    <mergeCell ref="A191:A192"/>
-    <mergeCell ref="C191:C192"/>
-    <mergeCell ref="A194:A195"/>
-    <mergeCell ref="C194:C195"/>
-    <mergeCell ref="A197:A198"/>
-    <mergeCell ref="C197:C198"/>
-    <mergeCell ref="A184:A185"/>
-    <mergeCell ref="B184:B185"/>
-    <mergeCell ref="A186:A188"/>
-    <mergeCell ref="B186:B188"/>
-    <mergeCell ref="A189:A190"/>
-    <mergeCell ref="C189:C190"/>
-    <mergeCell ref="A174:A175"/>
-    <mergeCell ref="C174:C175"/>
-    <mergeCell ref="A176:A177"/>
-    <mergeCell ref="C176:C177"/>
-    <mergeCell ref="A180:A181"/>
-    <mergeCell ref="A182:A183"/>
-    <mergeCell ref="B182:B183"/>
-    <mergeCell ref="A148:A160"/>
-    <mergeCell ref="A161:A164"/>
-    <mergeCell ref="A165:A169"/>
-    <mergeCell ref="B165:B169"/>
-    <mergeCell ref="A171:A172"/>
-    <mergeCell ref="C171:C172"/>
-    <mergeCell ref="A137:A138"/>
-    <mergeCell ref="A139:A140"/>
-    <mergeCell ref="A141:A142"/>
-    <mergeCell ref="A143:A145"/>
-    <mergeCell ref="A146:A147"/>
-    <mergeCell ref="C146:C147"/>
-    <mergeCell ref="A127:A128"/>
-    <mergeCell ref="C127:C128"/>
-    <mergeCell ref="A129:A136"/>
-    <mergeCell ref="A59:A61"/>
-    <mergeCell ref="A70:A73"/>
-    <mergeCell ref="A97:A100"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="A115:A118"/>
-    <mergeCell ref="A123:A124"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A31:A32"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="A50:A56"/>
-    <mergeCell ref="C123:C124"/>
-    <mergeCell ref="A125:A126"/>
-    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="A287:A288"/>
+    <mergeCell ref="A289:A290"/>
+    <mergeCell ref="A308:A312"/>
+    <mergeCell ref="A277:A278"/>
+    <mergeCell ref="C277:C278"/>
+    <mergeCell ref="A279:A280"/>
+    <mergeCell ref="C279:C280"/>
+    <mergeCell ref="A284:A285"/>
+    <mergeCell ref="C284:C285"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>